<commit_message>
sua Record of Changes
</commit_message>
<xml_diff>
--- a/docs/ProjectCode_TestPlan.xlsx
+++ b/docs/ProjectCode_TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\quản trị dự án CNTT\Qu-n-l-d-n-CNTT\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5B6B89-4B4C-4469-9B6C-AA7A0E67D58C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279E9C18-CDF5-4273-A399-CB1939FF1FBD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="15375" windowHeight="8325" tabRatio="848" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="324">
   <si>
     <t>Estimation &amp; Schedule</t>
   </si>
@@ -1043,6 +1043,12 @@
   </si>
   <si>
     <t>A document summarizing testing activities and results. It also contains an evaluation of the corresponding test items</t>
+  </si>
+  <si>
+    <t>&lt;2019/12/04&gt;</t>
+  </si>
+  <si>
+    <t>nhóm 12</t>
   </si>
 </sst>
 </file>
@@ -1590,19 +1596,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1616,20 +1616,20 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1643,29 +1643,35 @@
     <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1682,6 +1688,10 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1693,10 +1703,6 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -9916,7 +9922,7 @@
   </sheetPr>
   <dimension ref="B1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
       <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
@@ -12338,22 +12344,22 @@
     </row>
     <row r="3" spans="1:50" s="29" customFormat="1">
       <c r="A3" s="28"/>
-      <c r="B3" s="142" t="s">
+      <c r="B3" s="141" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="175" t="s">
+      <c r="C3" s="141"/>
+      <c r="D3" s="171" t="s">
         <v>281</v>
       </c>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="175"/>
-      <c r="I3" s="175"/>
-      <c r="J3" s="175"/>
-      <c r="K3" s="175"/>
-      <c r="L3" s="175"/>
-      <c r="M3" s="175"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="171"/>
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="171"/>
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
       <c r="P3" s="51"/>
@@ -12411,44 +12417,44 @@
       <c r="K4" s="169"/>
       <c r="L4" s="169"/>
       <c r="M4" s="169"/>
-      <c r="N4" s="174" t="s">
+      <c r="N4" s="170" t="s">
         <v>283</v>
       </c>
-      <c r="O4" s="174"/>
-      <c r="P4" s="174"/>
-      <c r="Q4" s="174"/>
-      <c r="R4" s="174"/>
-      <c r="S4" s="174"/>
-      <c r="T4" s="174"/>
-      <c r="U4" s="174"/>
-      <c r="V4" s="174"/>
-      <c r="W4" s="174"/>
-      <c r="X4" s="174"/>
-      <c r="Y4" s="174"/>
-      <c r="Z4" s="174"/>
-      <c r="AA4" s="174"/>
-      <c r="AB4" s="174"/>
-      <c r="AC4" s="174"/>
-      <c r="AD4" s="174"/>
-      <c r="AE4" s="174"/>
-      <c r="AF4" s="174"/>
-      <c r="AG4" s="174"/>
-      <c r="AH4" s="174"/>
-      <c r="AI4" s="174"/>
-      <c r="AJ4" s="174"/>
-      <c r="AK4" s="174"/>
-      <c r="AL4" s="174"/>
-      <c r="AM4" s="174"/>
-      <c r="AN4" s="174"/>
-      <c r="AO4" s="174"/>
-      <c r="AP4" s="174"/>
-      <c r="AQ4" s="174"/>
-      <c r="AR4" s="174"/>
-      <c r="AS4" s="174"/>
-      <c r="AT4" s="174"/>
-      <c r="AU4" s="174"/>
-      <c r="AV4" s="174"/>
-      <c r="AW4" s="174"/>
+      <c r="O4" s="170"/>
+      <c r="P4" s="170"/>
+      <c r="Q4" s="170"/>
+      <c r="R4" s="170"/>
+      <c r="S4" s="170"/>
+      <c r="T4" s="170"/>
+      <c r="U4" s="170"/>
+      <c r="V4" s="170"/>
+      <c r="W4" s="170"/>
+      <c r="X4" s="170"/>
+      <c r="Y4" s="170"/>
+      <c r="Z4" s="170"/>
+      <c r="AA4" s="170"/>
+      <c r="AB4" s="170"/>
+      <c r="AC4" s="170"/>
+      <c r="AD4" s="170"/>
+      <c r="AE4" s="170"/>
+      <c r="AF4" s="170"/>
+      <c r="AG4" s="170"/>
+      <c r="AH4" s="170"/>
+      <c r="AI4" s="170"/>
+      <c r="AJ4" s="170"/>
+      <c r="AK4" s="170"/>
+      <c r="AL4" s="170"/>
+      <c r="AM4" s="170"/>
+      <c r="AN4" s="170"/>
+      <c r="AO4" s="170"/>
+      <c r="AP4" s="170"/>
+      <c r="AQ4" s="170"/>
+      <c r="AR4" s="170"/>
+      <c r="AS4" s="170"/>
+      <c r="AT4" s="170"/>
+      <c r="AU4" s="170"/>
+      <c r="AV4" s="170"/>
+      <c r="AW4" s="170"/>
     </row>
     <row r="5" spans="1:50" s="29" customFormat="1" ht="14.25" customHeight="1">
       <c r="B5" s="168" t="s">
@@ -12467,44 +12473,44 @@
       <c r="K5" s="169"/>
       <c r="L5" s="169"/>
       <c r="M5" s="169"/>
-      <c r="N5" s="174" t="s">
+      <c r="N5" s="170" t="s">
         <v>285</v>
       </c>
-      <c r="O5" s="174"/>
-      <c r="P5" s="174"/>
-      <c r="Q5" s="174"/>
-      <c r="R5" s="174"/>
-      <c r="S5" s="174"/>
-      <c r="T5" s="174"/>
-      <c r="U5" s="174"/>
-      <c r="V5" s="174"/>
-      <c r="W5" s="174"/>
-      <c r="X5" s="174"/>
-      <c r="Y5" s="174"/>
-      <c r="Z5" s="174"/>
-      <c r="AA5" s="174"/>
-      <c r="AB5" s="174"/>
-      <c r="AC5" s="174"/>
-      <c r="AD5" s="174"/>
-      <c r="AE5" s="174"/>
-      <c r="AF5" s="174"/>
-      <c r="AG5" s="174"/>
-      <c r="AH5" s="174"/>
-      <c r="AI5" s="174"/>
-      <c r="AJ5" s="174"/>
-      <c r="AK5" s="174"/>
-      <c r="AL5" s="174"/>
-      <c r="AM5" s="174"/>
-      <c r="AN5" s="174"/>
-      <c r="AO5" s="174"/>
-      <c r="AP5" s="174"/>
-      <c r="AQ5" s="174"/>
-      <c r="AR5" s="174"/>
-      <c r="AS5" s="174"/>
-      <c r="AT5" s="174"/>
-      <c r="AU5" s="174"/>
-      <c r="AV5" s="174"/>
-      <c r="AW5" s="174"/>
+      <c r="O5" s="170"/>
+      <c r="P5" s="170"/>
+      <c r="Q5" s="170"/>
+      <c r="R5" s="170"/>
+      <c r="S5" s="170"/>
+      <c r="T5" s="170"/>
+      <c r="U5" s="170"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
+      <c r="X5" s="170"/>
+      <c r="Y5" s="170"/>
+      <c r="Z5" s="170"/>
+      <c r="AA5" s="170"/>
+      <c r="AB5" s="170"/>
+      <c r="AC5" s="170"/>
+      <c r="AD5" s="170"/>
+      <c r="AE5" s="170"/>
+      <c r="AF5" s="170"/>
+      <c r="AG5" s="170"/>
+      <c r="AH5" s="170"/>
+      <c r="AI5" s="170"/>
+      <c r="AJ5" s="170"/>
+      <c r="AK5" s="170"/>
+      <c r="AL5" s="170"/>
+      <c r="AM5" s="170"/>
+      <c r="AN5" s="170"/>
+      <c r="AO5" s="170"/>
+      <c r="AP5" s="170"/>
+      <c r="AQ5" s="170"/>
+      <c r="AR5" s="170"/>
+      <c r="AS5" s="170"/>
+      <c r="AT5" s="170"/>
+      <c r="AU5" s="170"/>
+      <c r="AV5" s="170"/>
+      <c r="AW5" s="170"/>
     </row>
     <row r="6" spans="1:50" s="29" customFormat="1" ht="14.25" customHeight="1">
       <c r="B6" s="168" t="s">
@@ -12523,44 +12529,44 @@
       <c r="K6" s="169"/>
       <c r="L6" s="169"/>
       <c r="M6" s="169"/>
-      <c r="N6" s="174" t="s">
+      <c r="N6" s="170" t="s">
         <v>287</v>
       </c>
-      <c r="O6" s="174"/>
-      <c r="P6" s="174"/>
-      <c r="Q6" s="174"/>
-      <c r="R6" s="174"/>
-      <c r="S6" s="174"/>
-      <c r="T6" s="174"/>
-      <c r="U6" s="174"/>
-      <c r="V6" s="174"/>
-      <c r="W6" s="174"/>
-      <c r="X6" s="174"/>
-      <c r="Y6" s="174"/>
-      <c r="Z6" s="174"/>
-      <c r="AA6" s="174"/>
-      <c r="AB6" s="174"/>
-      <c r="AC6" s="174"/>
-      <c r="AD6" s="174"/>
-      <c r="AE6" s="174"/>
-      <c r="AF6" s="174"/>
-      <c r="AG6" s="174"/>
-      <c r="AH6" s="174"/>
-      <c r="AI6" s="174"/>
-      <c r="AJ6" s="174"/>
-      <c r="AK6" s="174"/>
-      <c r="AL6" s="174"/>
-      <c r="AM6" s="174"/>
-      <c r="AN6" s="174"/>
-      <c r="AO6" s="174"/>
-      <c r="AP6" s="174"/>
-      <c r="AQ6" s="174"/>
-      <c r="AR6" s="174"/>
-      <c r="AS6" s="174"/>
-      <c r="AT6" s="174"/>
-      <c r="AU6" s="174"/>
-      <c r="AV6" s="174"/>
-      <c r="AW6" s="174"/>
+      <c r="O6" s="170"/>
+      <c r="P6" s="170"/>
+      <c r="Q6" s="170"/>
+      <c r="R6" s="170"/>
+      <c r="S6" s="170"/>
+      <c r="T6" s="170"/>
+      <c r="U6" s="170"/>
+      <c r="V6" s="170"/>
+      <c r="W6" s="170"/>
+      <c r="X6" s="170"/>
+      <c r="Y6" s="170"/>
+      <c r="Z6" s="170"/>
+      <c r="AA6" s="170"/>
+      <c r="AB6" s="170"/>
+      <c r="AC6" s="170"/>
+      <c r="AD6" s="170"/>
+      <c r="AE6" s="170"/>
+      <c r="AF6" s="170"/>
+      <c r="AG6" s="170"/>
+      <c r="AH6" s="170"/>
+      <c r="AI6" s="170"/>
+      <c r="AJ6" s="170"/>
+      <c r="AK6" s="170"/>
+      <c r="AL6" s="170"/>
+      <c r="AM6" s="170"/>
+      <c r="AN6" s="170"/>
+      <c r="AO6" s="170"/>
+      <c r="AP6" s="170"/>
+      <c r="AQ6" s="170"/>
+      <c r="AR6" s="170"/>
+      <c r="AS6" s="170"/>
+      <c r="AT6" s="170"/>
+      <c r="AU6" s="170"/>
+      <c r="AV6" s="170"/>
+      <c r="AW6" s="170"/>
     </row>
     <row r="7" spans="1:50" s="29" customFormat="1" ht="14.25" customHeight="1">
       <c r="B7" s="168" t="s">
@@ -12579,100 +12585,100 @@
       <c r="K7" s="169"/>
       <c r="L7" s="169"/>
       <c r="M7" s="169"/>
-      <c r="N7" s="174" t="s">
+      <c r="N7" s="170" t="s">
         <v>289</v>
       </c>
-      <c r="O7" s="174"/>
-      <c r="P7" s="174"/>
-      <c r="Q7" s="174"/>
-      <c r="R7" s="174"/>
-      <c r="S7" s="174"/>
-      <c r="T7" s="174"/>
-      <c r="U7" s="174"/>
-      <c r="V7" s="174"/>
-      <c r="W7" s="174"/>
-      <c r="X7" s="174"/>
-      <c r="Y7" s="174"/>
-      <c r="Z7" s="174"/>
-      <c r="AA7" s="174"/>
-      <c r="AB7" s="174"/>
-      <c r="AC7" s="174"/>
-      <c r="AD7" s="174"/>
-      <c r="AE7" s="174"/>
-      <c r="AF7" s="174"/>
-      <c r="AG7" s="174"/>
-      <c r="AH7" s="174"/>
-      <c r="AI7" s="174"/>
-      <c r="AJ7" s="174"/>
-      <c r="AK7" s="174"/>
-      <c r="AL7" s="174"/>
-      <c r="AM7" s="174"/>
-      <c r="AN7" s="174"/>
-      <c r="AO7" s="174"/>
-      <c r="AP7" s="174"/>
-      <c r="AQ7" s="174"/>
-      <c r="AR7" s="174"/>
-      <c r="AS7" s="174"/>
-      <c r="AT7" s="174"/>
-      <c r="AU7" s="174"/>
-      <c r="AV7" s="174"/>
-      <c r="AW7" s="174"/>
+      <c r="O7" s="170"/>
+      <c r="P7" s="170"/>
+      <c r="Q7" s="170"/>
+      <c r="R7" s="170"/>
+      <c r="S7" s="170"/>
+      <c r="T7" s="170"/>
+      <c r="U7" s="170"/>
+      <c r="V7" s="170"/>
+      <c r="W7" s="170"/>
+      <c r="X7" s="170"/>
+      <c r="Y7" s="170"/>
+      <c r="Z7" s="170"/>
+      <c r="AA7" s="170"/>
+      <c r="AB7" s="170"/>
+      <c r="AC7" s="170"/>
+      <c r="AD7" s="170"/>
+      <c r="AE7" s="170"/>
+      <c r="AF7" s="170"/>
+      <c r="AG7" s="170"/>
+      <c r="AH7" s="170"/>
+      <c r="AI7" s="170"/>
+      <c r="AJ7" s="170"/>
+      <c r="AK7" s="170"/>
+      <c r="AL7" s="170"/>
+      <c r="AM7" s="170"/>
+      <c r="AN7" s="170"/>
+      <c r="AO7" s="170"/>
+      <c r="AP7" s="170"/>
+      <c r="AQ7" s="170"/>
+      <c r="AR7" s="170"/>
+      <c r="AS7" s="170"/>
+      <c r="AT7" s="170"/>
+      <c r="AU7" s="170"/>
+      <c r="AV7" s="170"/>
+      <c r="AW7" s="170"/>
     </row>
     <row r="8" spans="1:50" s="29" customFormat="1" ht="30.75" customHeight="1">
-      <c r="B8" s="170" t="s">
+      <c r="B8" s="172" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="170"/>
-      <c r="D8" s="171" t="s">
+      <c r="C8" s="172"/>
+      <c r="D8" s="173" t="s">
         <v>290</v>
       </c>
-      <c r="E8" s="171"/>
-      <c r="F8" s="171"/>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="171"/>
-      <c r="K8" s="171"/>
-      <c r="L8" s="171"/>
-      <c r="M8" s="171"/>
-      <c r="N8" s="172" t="s">
+      <c r="E8" s="173"/>
+      <c r="F8" s="173"/>
+      <c r="G8" s="173"/>
+      <c r="H8" s="173"/>
+      <c r="I8" s="173"/>
+      <c r="J8" s="173"/>
+      <c r="K8" s="173"/>
+      <c r="L8" s="173"/>
+      <c r="M8" s="173"/>
+      <c r="N8" s="174" t="s">
         <v>291</v>
       </c>
-      <c r="O8" s="172"/>
-      <c r="P8" s="172"/>
-      <c r="Q8" s="172"/>
-      <c r="R8" s="172"/>
-      <c r="S8" s="172"/>
-      <c r="T8" s="172"/>
-      <c r="U8" s="172"/>
-      <c r="V8" s="172"/>
-      <c r="W8" s="172"/>
-      <c r="X8" s="172"/>
-      <c r="Y8" s="172"/>
-      <c r="Z8" s="172"/>
-      <c r="AA8" s="172"/>
-      <c r="AB8" s="172"/>
-      <c r="AC8" s="172"/>
-      <c r="AD8" s="172"/>
-      <c r="AE8" s="172"/>
-      <c r="AF8" s="172"/>
-      <c r="AG8" s="172"/>
-      <c r="AH8" s="172"/>
-      <c r="AI8" s="172"/>
-      <c r="AJ8" s="172"/>
-      <c r="AK8" s="172"/>
-      <c r="AL8" s="172"/>
-      <c r="AM8" s="172"/>
-      <c r="AN8" s="172"/>
-      <c r="AO8" s="172"/>
-      <c r="AP8" s="172"/>
-      <c r="AQ8" s="172"/>
-      <c r="AR8" s="172"/>
-      <c r="AS8" s="172"/>
-      <c r="AT8" s="172"/>
-      <c r="AU8" s="172"/>
-      <c r="AV8" s="172"/>
-      <c r="AW8" s="172"/>
+      <c r="O8" s="174"/>
+      <c r="P8" s="174"/>
+      <c r="Q8" s="174"/>
+      <c r="R8" s="174"/>
+      <c r="S8" s="174"/>
+      <c r="T8" s="174"/>
+      <c r="U8" s="174"/>
+      <c r="V8" s="174"/>
+      <c r="W8" s="174"/>
+      <c r="X8" s="174"/>
+      <c r="Y8" s="174"/>
+      <c r="Z8" s="174"/>
+      <c r="AA8" s="174"/>
+      <c r="AB8" s="174"/>
+      <c r="AC8" s="174"/>
+      <c r="AD8" s="174"/>
+      <c r="AE8" s="174"/>
+      <c r="AF8" s="174"/>
+      <c r="AG8" s="174"/>
+      <c r="AH8" s="174"/>
+      <c r="AI8" s="174"/>
+      <c r="AJ8" s="174"/>
+      <c r="AK8" s="174"/>
+      <c r="AL8" s="174"/>
+      <c r="AM8" s="174"/>
+      <c r="AN8" s="174"/>
+      <c r="AO8" s="174"/>
+      <c r="AP8" s="174"/>
+      <c r="AQ8" s="174"/>
+      <c r="AR8" s="174"/>
+      <c r="AS8" s="174"/>
+      <c r="AT8" s="174"/>
+      <c r="AU8" s="174"/>
+      <c r="AV8" s="174"/>
+      <c r="AW8" s="174"/>
     </row>
     <row r="9" spans="1:50" s="29" customFormat="1" ht="14.25" customHeight="1">
       <c r="B9" s="168" t="s">
@@ -12731,60 +12737,60 @@
       <c r="AW9" s="158"/>
     </row>
     <row r="10" spans="1:50" s="29" customFormat="1" ht="29.25" customHeight="1">
-      <c r="B10" s="170" t="s">
+      <c r="B10" s="172" t="s">
         <v>295</v>
       </c>
-      <c r="C10" s="170"/>
-      <c r="D10" s="171" t="s">
+      <c r="C10" s="172"/>
+      <c r="D10" s="173" t="s">
         <v>296</v>
       </c>
-      <c r="E10" s="171"/>
-      <c r="F10" s="171"/>
-      <c r="G10" s="171"/>
-      <c r="H10" s="171"/>
-      <c r="I10" s="171"/>
-      <c r="J10" s="171"/>
-      <c r="K10" s="171"/>
-      <c r="L10" s="171"/>
-      <c r="M10" s="171"/>
-      <c r="N10" s="172" t="s">
+      <c r="E10" s="173"/>
+      <c r="F10" s="173"/>
+      <c r="G10" s="173"/>
+      <c r="H10" s="173"/>
+      <c r="I10" s="173"/>
+      <c r="J10" s="173"/>
+      <c r="K10" s="173"/>
+      <c r="L10" s="173"/>
+      <c r="M10" s="173"/>
+      <c r="N10" s="174" t="s">
         <v>297</v>
       </c>
-      <c r="O10" s="172"/>
-      <c r="P10" s="172"/>
-      <c r="Q10" s="172"/>
-      <c r="R10" s="172"/>
-      <c r="S10" s="172"/>
-      <c r="T10" s="172"/>
-      <c r="U10" s="172"/>
-      <c r="V10" s="172"/>
-      <c r="W10" s="172"/>
-      <c r="X10" s="172"/>
-      <c r="Y10" s="172"/>
-      <c r="Z10" s="172"/>
-      <c r="AA10" s="172"/>
-      <c r="AB10" s="172"/>
-      <c r="AC10" s="172"/>
-      <c r="AD10" s="172"/>
-      <c r="AE10" s="172"/>
-      <c r="AF10" s="172"/>
-      <c r="AG10" s="172"/>
-      <c r="AH10" s="172"/>
-      <c r="AI10" s="172"/>
-      <c r="AJ10" s="172"/>
-      <c r="AK10" s="172"/>
-      <c r="AL10" s="172"/>
-      <c r="AM10" s="172"/>
-      <c r="AN10" s="172"/>
-      <c r="AO10" s="172"/>
-      <c r="AP10" s="172"/>
-      <c r="AQ10" s="172"/>
-      <c r="AR10" s="172"/>
-      <c r="AS10" s="172"/>
-      <c r="AT10" s="172"/>
-      <c r="AU10" s="172"/>
-      <c r="AV10" s="172"/>
-      <c r="AW10" s="172"/>
+      <c r="O10" s="174"/>
+      <c r="P10" s="174"/>
+      <c r="Q10" s="174"/>
+      <c r="R10" s="174"/>
+      <c r="S10" s="174"/>
+      <c r="T10" s="174"/>
+      <c r="U10" s="174"/>
+      <c r="V10" s="174"/>
+      <c r="W10" s="174"/>
+      <c r="X10" s="174"/>
+      <c r="Y10" s="174"/>
+      <c r="Z10" s="174"/>
+      <c r="AA10" s="174"/>
+      <c r="AB10" s="174"/>
+      <c r="AC10" s="174"/>
+      <c r="AD10" s="174"/>
+      <c r="AE10" s="174"/>
+      <c r="AF10" s="174"/>
+      <c r="AG10" s="174"/>
+      <c r="AH10" s="174"/>
+      <c r="AI10" s="174"/>
+      <c r="AJ10" s="174"/>
+      <c r="AK10" s="174"/>
+      <c r="AL10" s="174"/>
+      <c r="AM10" s="174"/>
+      <c r="AN10" s="174"/>
+      <c r="AO10" s="174"/>
+      <c r="AP10" s="174"/>
+      <c r="AQ10" s="174"/>
+      <c r="AR10" s="174"/>
+      <c r="AS10" s="174"/>
+      <c r="AT10" s="174"/>
+      <c r="AU10" s="174"/>
+      <c r="AV10" s="174"/>
+      <c r="AW10" s="174"/>
     </row>
     <row r="11" spans="1:50" s="29" customFormat="1" ht="14.25" customHeight="1">
       <c r="B11" s="168" t="s">
@@ -12843,60 +12849,60 @@
       <c r="AW11" s="158"/>
     </row>
     <row r="12" spans="1:50" s="29" customFormat="1" ht="29.25" customHeight="1">
-      <c r="B12" s="170" t="s">
+      <c r="B12" s="172" t="s">
         <v>301</v>
       </c>
-      <c r="C12" s="170"/>
-      <c r="D12" s="171" t="s">
+      <c r="C12" s="172"/>
+      <c r="D12" s="173" t="s">
         <v>302</v>
       </c>
-      <c r="E12" s="171"/>
-      <c r="F12" s="171"/>
-      <c r="G12" s="171"/>
-      <c r="H12" s="171"/>
-      <c r="I12" s="171"/>
-      <c r="J12" s="171"/>
-      <c r="K12" s="171"/>
-      <c r="L12" s="171"/>
-      <c r="M12" s="171"/>
-      <c r="N12" s="172" t="s">
+      <c r="E12" s="173"/>
+      <c r="F12" s="173"/>
+      <c r="G12" s="173"/>
+      <c r="H12" s="173"/>
+      <c r="I12" s="173"/>
+      <c r="J12" s="173"/>
+      <c r="K12" s="173"/>
+      <c r="L12" s="173"/>
+      <c r="M12" s="173"/>
+      <c r="N12" s="174" t="s">
         <v>303</v>
       </c>
-      <c r="O12" s="172"/>
-      <c r="P12" s="172"/>
-      <c r="Q12" s="172"/>
-      <c r="R12" s="172"/>
-      <c r="S12" s="172"/>
-      <c r="T12" s="172"/>
-      <c r="U12" s="172"/>
-      <c r="V12" s="172"/>
-      <c r="W12" s="172"/>
-      <c r="X12" s="172"/>
-      <c r="Y12" s="172"/>
-      <c r="Z12" s="172"/>
-      <c r="AA12" s="172"/>
-      <c r="AB12" s="172"/>
-      <c r="AC12" s="172"/>
-      <c r="AD12" s="172"/>
-      <c r="AE12" s="172"/>
-      <c r="AF12" s="172"/>
-      <c r="AG12" s="172"/>
-      <c r="AH12" s="172"/>
-      <c r="AI12" s="172"/>
-      <c r="AJ12" s="172"/>
-      <c r="AK12" s="172"/>
-      <c r="AL12" s="172"/>
-      <c r="AM12" s="172"/>
-      <c r="AN12" s="172"/>
-      <c r="AO12" s="172"/>
-      <c r="AP12" s="172"/>
-      <c r="AQ12" s="172"/>
-      <c r="AR12" s="172"/>
-      <c r="AS12" s="172"/>
-      <c r="AT12" s="172"/>
-      <c r="AU12" s="172"/>
-      <c r="AV12" s="172"/>
-      <c r="AW12" s="172"/>
+      <c r="O12" s="174"/>
+      <c r="P12" s="174"/>
+      <c r="Q12" s="174"/>
+      <c r="R12" s="174"/>
+      <c r="S12" s="174"/>
+      <c r="T12" s="174"/>
+      <c r="U12" s="174"/>
+      <c r="V12" s="174"/>
+      <c r="W12" s="174"/>
+      <c r="X12" s="174"/>
+      <c r="Y12" s="174"/>
+      <c r="Z12" s="174"/>
+      <c r="AA12" s="174"/>
+      <c r="AB12" s="174"/>
+      <c r="AC12" s="174"/>
+      <c r="AD12" s="174"/>
+      <c r="AE12" s="174"/>
+      <c r="AF12" s="174"/>
+      <c r="AG12" s="174"/>
+      <c r="AH12" s="174"/>
+      <c r="AI12" s="174"/>
+      <c r="AJ12" s="174"/>
+      <c r="AK12" s="174"/>
+      <c r="AL12" s="174"/>
+      <c r="AM12" s="174"/>
+      <c r="AN12" s="174"/>
+      <c r="AO12" s="174"/>
+      <c r="AP12" s="174"/>
+      <c r="AQ12" s="174"/>
+      <c r="AR12" s="174"/>
+      <c r="AS12" s="174"/>
+      <c r="AT12" s="174"/>
+      <c r="AU12" s="174"/>
+      <c r="AV12" s="174"/>
+      <c r="AW12" s="174"/>
     </row>
     <row r="13" spans="1:50" s="29" customFormat="1" ht="14.25" customHeight="1">
       <c r="B13" s="168" t="s">
@@ -12971,44 +12977,44 @@
       <c r="K14" s="169"/>
       <c r="L14" s="169"/>
       <c r="M14" s="169"/>
-      <c r="N14" s="173" t="s">
+      <c r="N14" s="175" t="s">
         <v>309</v>
       </c>
-      <c r="O14" s="173"/>
-      <c r="P14" s="173"/>
-      <c r="Q14" s="173"/>
-      <c r="R14" s="173"/>
-      <c r="S14" s="173"/>
-      <c r="T14" s="173"/>
-      <c r="U14" s="173"/>
-      <c r="V14" s="173"/>
-      <c r="W14" s="173"/>
-      <c r="X14" s="173"/>
-      <c r="Y14" s="173"/>
-      <c r="Z14" s="173"/>
-      <c r="AA14" s="173"/>
-      <c r="AB14" s="173"/>
-      <c r="AC14" s="173"/>
-      <c r="AD14" s="173"/>
-      <c r="AE14" s="173"/>
-      <c r="AF14" s="173"/>
-      <c r="AG14" s="173"/>
-      <c r="AH14" s="173"/>
-      <c r="AI14" s="173"/>
-      <c r="AJ14" s="173"/>
-      <c r="AK14" s="173"/>
-      <c r="AL14" s="173"/>
-      <c r="AM14" s="173"/>
-      <c r="AN14" s="173"/>
-      <c r="AO14" s="173"/>
-      <c r="AP14" s="173"/>
-      <c r="AQ14" s="173"/>
-      <c r="AR14" s="173"/>
-      <c r="AS14" s="173"/>
-      <c r="AT14" s="173"/>
-      <c r="AU14" s="173"/>
-      <c r="AV14" s="173"/>
-      <c r="AW14" s="173"/>
+      <c r="O14" s="175"/>
+      <c r="P14" s="175"/>
+      <c r="Q14" s="175"/>
+      <c r="R14" s="175"/>
+      <c r="S14" s="175"/>
+      <c r="T14" s="175"/>
+      <c r="U14" s="175"/>
+      <c r="V14" s="175"/>
+      <c r="W14" s="175"/>
+      <c r="X14" s="175"/>
+      <c r="Y14" s="175"/>
+      <c r="Z14" s="175"/>
+      <c r="AA14" s="175"/>
+      <c r="AB14" s="175"/>
+      <c r="AC14" s="175"/>
+      <c r="AD14" s="175"/>
+      <c r="AE14" s="175"/>
+      <c r="AF14" s="175"/>
+      <c r="AG14" s="175"/>
+      <c r="AH14" s="175"/>
+      <c r="AI14" s="175"/>
+      <c r="AJ14" s="175"/>
+      <c r="AK14" s="175"/>
+      <c r="AL14" s="175"/>
+      <c r="AM14" s="175"/>
+      <c r="AN14" s="175"/>
+      <c r="AO14" s="175"/>
+      <c r="AP14" s="175"/>
+      <c r="AQ14" s="175"/>
+      <c r="AR14" s="175"/>
+      <c r="AS14" s="175"/>
+      <c r="AT14" s="175"/>
+      <c r="AU14" s="175"/>
+      <c r="AV14" s="175"/>
+      <c r="AW14" s="175"/>
     </row>
     <row r="15" spans="1:50" s="29" customFormat="1" ht="14.25" customHeight="1">
       <c r="B15" s="168" t="s">
@@ -13067,60 +13073,60 @@
       <c r="AW15" s="158"/>
     </row>
     <row r="16" spans="1:50" s="88" customFormat="1" ht="43.5" customHeight="1">
-      <c r="B16" s="170" t="s">
+      <c r="B16" s="172" t="s">
         <v>313</v>
       </c>
-      <c r="C16" s="170"/>
-      <c r="D16" s="171" t="s">
+      <c r="C16" s="172"/>
+      <c r="D16" s="173" t="s">
         <v>314</v>
       </c>
-      <c r="E16" s="171"/>
-      <c r="F16" s="171"/>
-      <c r="G16" s="171"/>
-      <c r="H16" s="171"/>
-      <c r="I16" s="171"/>
-      <c r="J16" s="171"/>
-      <c r="K16" s="171"/>
-      <c r="L16" s="171"/>
-      <c r="M16" s="171"/>
-      <c r="N16" s="172" t="s">
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
+      <c r="L16" s="173"/>
+      <c r="M16" s="173"/>
+      <c r="N16" s="174" t="s">
         <v>315</v>
       </c>
-      <c r="O16" s="172"/>
-      <c r="P16" s="172"/>
-      <c r="Q16" s="172"/>
-      <c r="R16" s="172"/>
-      <c r="S16" s="172"/>
-      <c r="T16" s="172"/>
-      <c r="U16" s="172"/>
-      <c r="V16" s="172"/>
-      <c r="W16" s="172"/>
-      <c r="X16" s="172"/>
-      <c r="Y16" s="172"/>
-      <c r="Z16" s="172"/>
-      <c r="AA16" s="172"/>
-      <c r="AB16" s="172"/>
-      <c r="AC16" s="172"/>
-      <c r="AD16" s="172"/>
-      <c r="AE16" s="172"/>
-      <c r="AF16" s="172"/>
-      <c r="AG16" s="172"/>
-      <c r="AH16" s="172"/>
-      <c r="AI16" s="172"/>
-      <c r="AJ16" s="172"/>
-      <c r="AK16" s="172"/>
-      <c r="AL16" s="172"/>
-      <c r="AM16" s="172"/>
-      <c r="AN16" s="172"/>
-      <c r="AO16" s="172"/>
-      <c r="AP16" s="172"/>
-      <c r="AQ16" s="172"/>
-      <c r="AR16" s="172"/>
-      <c r="AS16" s="172"/>
-      <c r="AT16" s="172"/>
-      <c r="AU16" s="172"/>
-      <c r="AV16" s="172"/>
-      <c r="AW16" s="172"/>
+      <c r="O16" s="174"/>
+      <c r="P16" s="174"/>
+      <c r="Q16" s="174"/>
+      <c r="R16" s="174"/>
+      <c r="S16" s="174"/>
+      <c r="T16" s="174"/>
+      <c r="U16" s="174"/>
+      <c r="V16" s="174"/>
+      <c r="W16" s="174"/>
+      <c r="X16" s="174"/>
+      <c r="Y16" s="174"/>
+      <c r="Z16" s="174"/>
+      <c r="AA16" s="174"/>
+      <c r="AB16" s="174"/>
+      <c r="AC16" s="174"/>
+      <c r="AD16" s="174"/>
+      <c r="AE16" s="174"/>
+      <c r="AF16" s="174"/>
+      <c r="AG16" s="174"/>
+      <c r="AH16" s="174"/>
+      <c r="AI16" s="174"/>
+      <c r="AJ16" s="174"/>
+      <c r="AK16" s="174"/>
+      <c r="AL16" s="174"/>
+      <c r="AM16" s="174"/>
+      <c r="AN16" s="174"/>
+      <c r="AO16" s="174"/>
+      <c r="AP16" s="174"/>
+      <c r="AQ16" s="174"/>
+      <c r="AR16" s="174"/>
+      <c r="AS16" s="174"/>
+      <c r="AT16" s="174"/>
+      <c r="AU16" s="174"/>
+      <c r="AV16" s="174"/>
+      <c r="AW16" s="174"/>
     </row>
     <row r="17" spans="2:49" s="29" customFormat="1" ht="14.25" customHeight="1">
       <c r="B17" s="168" t="s">
@@ -13930,74 +13936,6 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:M5"/>
-    <mergeCell ref="N5:AW5"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:M4"/>
-    <mergeCell ref="N4:AW4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:M6"/>
-    <mergeCell ref="N6:AW6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="N7:AW7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:M8"/>
-    <mergeCell ref="N8:AW8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:M9"/>
-    <mergeCell ref="N9:AW9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:M10"/>
-    <mergeCell ref="N10:AW10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:M11"/>
-    <mergeCell ref="N11:AW11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:M12"/>
-    <mergeCell ref="N12:AW12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:M13"/>
-    <mergeCell ref="N13:AW13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:M14"/>
-    <mergeCell ref="N14:AW14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:M15"/>
-    <mergeCell ref="N15:AW15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:M16"/>
-    <mergeCell ref="N16:AW16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:M17"/>
-    <mergeCell ref="N17:AW17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:M18"/>
-    <mergeCell ref="N18:AW18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:M19"/>
-    <mergeCell ref="N19:AW19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:M20"/>
-    <mergeCell ref="N20:AW20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:M21"/>
-    <mergeCell ref="N21:AW21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:M22"/>
-    <mergeCell ref="N22:AW22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:M23"/>
-    <mergeCell ref="N23:AW23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:M24"/>
-    <mergeCell ref="N24:AW24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:M25"/>
-    <mergeCell ref="N25:AW25"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="D28:M28"/>
     <mergeCell ref="N28:AW28"/>
@@ -14007,6 +13945,74 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:M27"/>
     <mergeCell ref="N27:AW27"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:M24"/>
+    <mergeCell ref="N24:AW24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:M25"/>
+    <mergeCell ref="N25:AW25"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:M22"/>
+    <mergeCell ref="N22:AW22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:M23"/>
+    <mergeCell ref="N23:AW23"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:M20"/>
+    <mergeCell ref="N20:AW20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:M21"/>
+    <mergeCell ref="N21:AW21"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:M18"/>
+    <mergeCell ref="N18:AW18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:M19"/>
+    <mergeCell ref="N19:AW19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:M16"/>
+    <mergeCell ref="N16:AW16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:M17"/>
+    <mergeCell ref="N17:AW17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:M14"/>
+    <mergeCell ref="N14:AW14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:M15"/>
+    <mergeCell ref="N15:AW15"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:M12"/>
+    <mergeCell ref="N12:AW12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:M13"/>
+    <mergeCell ref="N13:AW13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:M10"/>
+    <mergeCell ref="N10:AW10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:M11"/>
+    <mergeCell ref="N11:AW11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:M8"/>
+    <mergeCell ref="N8:AW8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:M9"/>
+    <mergeCell ref="N9:AW9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:M6"/>
+    <mergeCell ref="N6:AW6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="N7:AW7"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:M5"/>
+    <mergeCell ref="N5:AW5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:M4"/>
+    <mergeCell ref="N4:AW4"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AR29:AW31" xr:uid="{00000000-0002-0000-0B00-000000000000}">
@@ -14027,8 +14033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:AX25"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -14279,7 +14285,7 @@
     </row>
     <row r="9" spans="2:50">
       <c r="B9" s="14" t="s">
-        <v>10</v>
+        <v>322</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>11</v>
@@ -14291,7 +14297,9 @@
       <c r="F9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="15" t="s">
+        <v>323</v>
+      </c>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
     </row>
@@ -16595,107 +16603,107 @@
     </row>
     <row r="3" spans="1:50" s="29" customFormat="1" ht="12.75" customHeight="1">
       <c r="A3" s="28"/>
-      <c r="B3" s="143" t="s">
+      <c r="B3" s="140" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143"/>
-      <c r="K3" s="143"/>
-      <c r="L3" s="143"/>
-      <c r="M3" s="143"/>
-      <c r="N3" s="143"/>
-      <c r="O3" s="143"/>
-      <c r="P3" s="143"/>
-      <c r="Q3" s="143"/>
-      <c r="R3" s="143"/>
-      <c r="S3" s="143"/>
-      <c r="T3" s="143"/>
-      <c r="U3" s="143"/>
-      <c r="V3" s="143"/>
-      <c r="W3" s="143"/>
-      <c r="X3" s="143"/>
-      <c r="Y3" s="143"/>
-      <c r="Z3" s="143"/>
-      <c r="AA3" s="143"/>
-      <c r="AB3" s="143"/>
-      <c r="AC3" s="143"/>
-      <c r="AD3" s="143"/>
-      <c r="AE3" s="143"/>
-      <c r="AF3" s="143"/>
-      <c r="AG3" s="143"/>
-      <c r="AH3" s="143"/>
-      <c r="AI3" s="143"/>
-      <c r="AJ3" s="143"/>
-      <c r="AK3" s="143"/>
-      <c r="AL3" s="143"/>
-      <c r="AM3" s="143"/>
-      <c r="AN3" s="143"/>
-      <c r="AO3" s="143"/>
-      <c r="AP3" s="143"/>
-      <c r="AQ3" s="143"/>
-      <c r="AR3" s="143"/>
-      <c r="AS3" s="143"/>
-      <c r="AT3" s="143"/>
-      <c r="AU3" s="143"/>
-      <c r="AV3" s="143"/>
-      <c r="AW3" s="143"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="140"/>
+      <c r="M3" s="140"/>
+      <c r="N3" s="140"/>
+      <c r="O3" s="140"/>
+      <c r="P3" s="140"/>
+      <c r="Q3" s="140"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="140"/>
+      <c r="T3" s="140"/>
+      <c r="U3" s="140"/>
+      <c r="V3" s="140"/>
+      <c r="W3" s="140"/>
+      <c r="X3" s="140"/>
+      <c r="Y3" s="140"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="140"/>
+      <c r="AB3" s="140"/>
+      <c r="AC3" s="140"/>
+      <c r="AD3" s="140"/>
+      <c r="AE3" s="140"/>
+      <c r="AF3" s="140"/>
+      <c r="AG3" s="140"/>
+      <c r="AH3" s="140"/>
+      <c r="AI3" s="140"/>
+      <c r="AJ3" s="140"/>
+      <c r="AK3" s="140"/>
+      <c r="AL3" s="140"/>
+      <c r="AM3" s="140"/>
+      <c r="AN3" s="140"/>
+      <c r="AO3" s="140"/>
+      <c r="AP3" s="140"/>
+      <c r="AQ3" s="140"/>
+      <c r="AR3" s="140"/>
+      <c r="AS3" s="140"/>
+      <c r="AT3" s="140"/>
+      <c r="AU3" s="140"/>
+      <c r="AV3" s="140"/>
+      <c r="AW3" s="140"/>
       <c r="AX3" s="40"/>
     </row>
     <row r="4" spans="1:50" ht="13.5" customHeight="1">
-      <c r="B4" s="143"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
-      <c r="G4" s="143"/>
-      <c r="H4" s="143"/>
-      <c r="I4" s="143"/>
-      <c r="J4" s="143"/>
-      <c r="K4" s="143"/>
-      <c r="L4" s="143"/>
-      <c r="M4" s="143"/>
-      <c r="N4" s="143"/>
-      <c r="O4" s="143"/>
-      <c r="P4" s="143"/>
-      <c r="Q4" s="143"/>
-      <c r="R4" s="143"/>
-      <c r="S4" s="143"/>
-      <c r="T4" s="143"/>
-      <c r="U4" s="143"/>
-      <c r="V4" s="143"/>
-      <c r="W4" s="143"/>
-      <c r="X4" s="143"/>
-      <c r="Y4" s="143"/>
-      <c r="Z4" s="143"/>
-      <c r="AA4" s="143"/>
-      <c r="AB4" s="143"/>
-      <c r="AC4" s="143"/>
-      <c r="AD4" s="143"/>
-      <c r="AE4" s="143"/>
-      <c r="AF4" s="143"/>
-      <c r="AG4" s="143"/>
-      <c r="AH4" s="143"/>
-      <c r="AI4" s="143"/>
-      <c r="AJ4" s="143"/>
-      <c r="AK4" s="143"/>
-      <c r="AL4" s="143"/>
-      <c r="AM4" s="143"/>
-      <c r="AN4" s="143"/>
-      <c r="AO4" s="143"/>
-      <c r="AP4" s="143"/>
-      <c r="AQ4" s="143"/>
-      <c r="AR4" s="143"/>
-      <c r="AS4" s="143"/>
-      <c r="AT4" s="143"/>
-      <c r="AU4" s="143"/>
-      <c r="AV4" s="143"/>
-      <c r="AW4" s="143"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="140"/>
+      <c r="M4" s="140"/>
+      <c r="N4" s="140"/>
+      <c r="O4" s="140"/>
+      <c r="P4" s="140"/>
+      <c r="Q4" s="140"/>
+      <c r="R4" s="140"/>
+      <c r="S4" s="140"/>
+      <c r="T4" s="140"/>
+      <c r="U4" s="140"/>
+      <c r="V4" s="140"/>
+      <c r="W4" s="140"/>
+      <c r="X4" s="140"/>
+      <c r="Y4" s="140"/>
+      <c r="Z4" s="140"/>
+      <c r="AA4" s="140"/>
+      <c r="AB4" s="140"/>
+      <c r="AC4" s="140"/>
+      <c r="AD4" s="140"/>
+      <c r="AE4" s="140"/>
+      <c r="AF4" s="140"/>
+      <c r="AG4" s="140"/>
+      <c r="AH4" s="140"/>
+      <c r="AI4" s="140"/>
+      <c r="AJ4" s="140"/>
+      <c r="AK4" s="140"/>
+      <c r="AL4" s="140"/>
+      <c r="AM4" s="140"/>
+      <c r="AN4" s="140"/>
+      <c r="AO4" s="140"/>
+      <c r="AP4" s="140"/>
+      <c r="AQ4" s="140"/>
+      <c r="AR4" s="140"/>
+      <c r="AS4" s="140"/>
+      <c r="AT4" s="140"/>
+      <c r="AU4" s="140"/>
+      <c r="AV4" s="140"/>
+      <c r="AW4" s="140"/>
       <c r="AX4" s="40"/>
     </row>
     <row r="5" spans="1:50" ht="13.5" customHeight="1">
@@ -17100,39 +17108,39 @@
     </row>
     <row r="17" spans="1:50" s="48" customFormat="1">
       <c r="A17" s="19"/>
-      <c r="B17" s="142" t="s">
+      <c r="B17" s="141" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="142"/>
-      <c r="D17" s="142" t="s">
+      <c r="C17" s="141"/>
+      <c r="D17" s="141" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="142"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="142"/>
-      <c r="H17" s="142"/>
-      <c r="I17" s="142"/>
-      <c r="J17" s="142"/>
-      <c r="K17" s="142" t="s">
+      <c r="E17" s="141"/>
+      <c r="F17" s="141"/>
+      <c r="G17" s="141"/>
+      <c r="H17" s="141"/>
+      <c r="I17" s="141"/>
+      <c r="J17" s="141"/>
+      <c r="K17" s="141" t="s">
         <v>88</v>
       </c>
-      <c r="L17" s="142"/>
-      <c r="M17" s="142"/>
-      <c r="N17" s="142"/>
-      <c r="O17" s="142"/>
-      <c r="P17" s="142"/>
-      <c r="Q17" s="142"/>
-      <c r="R17" s="142"/>
-      <c r="S17" s="142"/>
-      <c r="T17" s="142"/>
-      <c r="U17" s="142"/>
-      <c r="V17" s="142"/>
-      <c r="W17" s="142"/>
-      <c r="X17" s="142"/>
-      <c r="Y17" s="142"/>
-      <c r="Z17" s="142"/>
-      <c r="AA17" s="142"/>
-      <c r="AB17" s="142"/>
+      <c r="L17" s="141"/>
+      <c r="M17" s="141"/>
+      <c r="N17" s="141"/>
+      <c r="O17" s="141"/>
+      <c r="P17" s="141"/>
+      <c r="Q17" s="141"/>
+      <c r="R17" s="141"/>
+      <c r="S17" s="141"/>
+      <c r="T17" s="141"/>
+      <c r="U17" s="141"/>
+      <c r="V17" s="141"/>
+      <c r="W17" s="141"/>
+      <c r="X17" s="141"/>
+      <c r="Y17" s="141"/>
+      <c r="Z17" s="141"/>
+      <c r="AA17" s="141"/>
+      <c r="AB17" s="141"/>
       <c r="AC17" s="19"/>
       <c r="AD17" s="19"/>
       <c r="AE17" s="19"/>
@@ -17158,39 +17166,39 @@
     </row>
     <row r="18" spans="1:50">
       <c r="A18" s="48"/>
-      <c r="B18" s="144" t="s">
+      <c r="B18" s="142" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="144"/>
-      <c r="D18" s="145" t="s">
+      <c r="C18" s="142"/>
+      <c r="D18" s="143" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="145"/>
-      <c r="F18" s="145"/>
-      <c r="G18" s="145"/>
-      <c r="H18" s="145"/>
-      <c r="I18" s="145"/>
-      <c r="J18" s="145"/>
-      <c r="K18" s="146" t="s">
+      <c r="E18" s="143"/>
+      <c r="F18" s="143"/>
+      <c r="G18" s="143"/>
+      <c r="H18" s="143"/>
+      <c r="I18" s="143"/>
+      <c r="J18" s="143"/>
+      <c r="K18" s="144" t="s">
         <v>90</v>
       </c>
-      <c r="L18" s="146"/>
-      <c r="M18" s="146"/>
-      <c r="N18" s="146"/>
-      <c r="O18" s="146"/>
-      <c r="P18" s="146"/>
-      <c r="Q18" s="146"/>
-      <c r="R18" s="146"/>
-      <c r="S18" s="146"/>
-      <c r="T18" s="146"/>
-      <c r="U18" s="146"/>
-      <c r="V18" s="146"/>
-      <c r="W18" s="146"/>
-      <c r="X18" s="146"/>
-      <c r="Y18" s="146"/>
-      <c r="Z18" s="146"/>
-      <c r="AA18" s="146"/>
-      <c r="AB18" s="146"/>
+      <c r="L18" s="144"/>
+      <c r="M18" s="144"/>
+      <c r="N18" s="144"/>
+      <c r="O18" s="144"/>
+      <c r="P18" s="144"/>
+      <c r="Q18" s="144"/>
+      <c r="R18" s="144"/>
+      <c r="S18" s="144"/>
+      <c r="T18" s="144"/>
+      <c r="U18" s="144"/>
+      <c r="V18" s="144"/>
+      <c r="W18" s="144"/>
+      <c r="X18" s="144"/>
+      <c r="Y18" s="144"/>
+      <c r="Z18" s="144"/>
+      <c r="AA18" s="144"/>
+      <c r="AB18" s="144"/>
       <c r="AC18" s="48"/>
       <c r="AD18" s="48"/>
       <c r="AE18" s="48"/>
@@ -17215,39 +17223,39 @@
       <c r="AX18" s="48"/>
     </row>
     <row r="19" spans="1:50">
-      <c r="B19" s="144" t="s">
+      <c r="B19" s="142" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="144"/>
-      <c r="D19" s="147" t="s">
+      <c r="C19" s="142"/>
+      <c r="D19" s="145" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="147"/>
-      <c r="F19" s="147"/>
-      <c r="G19" s="147"/>
-      <c r="H19" s="147"/>
-      <c r="I19" s="147"/>
-      <c r="J19" s="147"/>
-      <c r="K19" s="146" t="s">
+      <c r="E19" s="145"/>
+      <c r="F19" s="145"/>
+      <c r="G19" s="145"/>
+      <c r="H19" s="145"/>
+      <c r="I19" s="145"/>
+      <c r="J19" s="145"/>
+      <c r="K19" s="144" t="s">
         <v>92</v>
       </c>
-      <c r="L19" s="146"/>
-      <c r="M19" s="146"/>
-      <c r="N19" s="146"/>
-      <c r="O19" s="146"/>
-      <c r="P19" s="146"/>
-      <c r="Q19" s="146"/>
-      <c r="R19" s="146"/>
-      <c r="S19" s="146"/>
-      <c r="T19" s="146"/>
-      <c r="U19" s="146"/>
-      <c r="V19" s="146"/>
-      <c r="W19" s="146"/>
-      <c r="X19" s="146"/>
-      <c r="Y19" s="146"/>
-      <c r="Z19" s="146"/>
-      <c r="AA19" s="146"/>
-      <c r="AB19" s="146"/>
+      <c r="L19" s="144"/>
+      <c r="M19" s="144"/>
+      <c r="N19" s="144"/>
+      <c r="O19" s="144"/>
+      <c r="P19" s="144"/>
+      <c r="Q19" s="144"/>
+      <c r="R19" s="144"/>
+      <c r="S19" s="144"/>
+      <c r="T19" s="144"/>
+      <c r="U19" s="144"/>
+      <c r="V19" s="144"/>
+      <c r="W19" s="144"/>
+      <c r="X19" s="144"/>
+      <c r="Y19" s="144"/>
+      <c r="Z19" s="144"/>
+      <c r="AA19" s="144"/>
+      <c r="AB19" s="144"/>
     </row>
     <row r="21" spans="1:50">
       <c r="A21" s="24" t="s">
@@ -17357,10 +17365,10 @@
     </row>
     <row r="23" spans="1:50">
       <c r="A23" s="19"/>
-      <c r="B23" s="142" t="s">
+      <c r="B23" s="141" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="142"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="50"/>
       <c r="E23" s="51"/>
       <c r="F23" s="51"/>
@@ -17414,10 +17422,10 @@
       <c r="AX23" s="19"/>
     </row>
     <row r="24" spans="1:50" s="29" customFormat="1">
-      <c r="B24" s="141">
+      <c r="B24" s="139">
         <v>1</v>
       </c>
-      <c r="C24" s="141"/>
+      <c r="C24" s="139"/>
       <c r="D24" s="57" t="s">
         <v>95</v>
       </c>
@@ -17463,10 +17471,10 @@
       <c r="AP24" s="63"/>
     </row>
     <row r="25" spans="1:50" s="29" customFormat="1">
-      <c r="B25" s="141">
+      <c r="B25" s="139">
         <v>2</v>
       </c>
-      <c r="C25" s="141"/>
+      <c r="C25" s="139"/>
       <c r="D25" s="57" t="s">
         <v>97</v>
       </c>
@@ -17512,10 +17520,10 @@
       <c r="AP25" s="63"/>
     </row>
     <row r="26" spans="1:50" s="29" customFormat="1">
-      <c r="B26" s="141">
+      <c r="B26" s="139">
         <v>3</v>
       </c>
-      <c r="C26" s="141"/>
+      <c r="C26" s="139"/>
       <c r="D26" s="57" t="s">
         <v>99</v>
       </c>
@@ -17561,10 +17569,10 @@
       <c r="AP26" s="63"/>
     </row>
     <row r="27" spans="1:50" s="29" customFormat="1">
-      <c r="B27" s="141">
+      <c r="B27" s="139">
         <v>4</v>
       </c>
-      <c r="C27" s="141"/>
+      <c r="C27" s="139"/>
       <c r="D27" s="57" t="s">
         <v>101</v>
       </c>
@@ -17596,10 +17604,10 @@
       <c r="AP27" s="63"/>
     </row>
     <row r="28" spans="1:50" s="29" customFormat="1">
-      <c r="B28" s="141">
+      <c r="B28" s="139">
         <v>5</v>
       </c>
-      <c r="C28" s="141"/>
+      <c r="C28" s="139"/>
       <c r="D28" s="57" t="s">
         <v>103</v>
       </c>
@@ -18202,33 +18210,33 @@
     </row>
     <row r="43" spans="1:50" s="29" customFormat="1">
       <c r="A43" s="19"/>
-      <c r="B43" s="142" t="s">
+      <c r="B43" s="141" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="142"/>
-      <c r="D43" s="142" t="s">
+      <c r="C43" s="141"/>
+      <c r="D43" s="141" t="s">
         <v>114</v>
       </c>
-      <c r="E43" s="142"/>
-      <c r="F43" s="142"/>
-      <c r="G43" s="142"/>
-      <c r="H43" s="142"/>
-      <c r="I43" s="142"/>
-      <c r="J43" s="142"/>
-      <c r="K43" s="142"/>
-      <c r="L43" s="142"/>
-      <c r="M43" s="142"/>
-      <c r="N43" s="142"/>
-      <c r="O43" s="142"/>
-      <c r="P43" s="142"/>
-      <c r="Q43" s="142"/>
-      <c r="R43" s="142"/>
-      <c r="S43" s="142"/>
-      <c r="T43" s="142"/>
-      <c r="U43" s="142"/>
-      <c r="V43" s="142"/>
-      <c r="W43" s="142"/>
-      <c r="X43" s="142"/>
+      <c r="E43" s="141"/>
+      <c r="F43" s="141"/>
+      <c r="G43" s="141"/>
+      <c r="H43" s="141"/>
+      <c r="I43" s="141"/>
+      <c r="J43" s="141"/>
+      <c r="K43" s="141"/>
+      <c r="L43" s="141"/>
+      <c r="M43" s="141"/>
+      <c r="N43" s="141"/>
+      <c r="O43" s="141"/>
+      <c r="P43" s="141"/>
+      <c r="Q43" s="141"/>
+      <c r="R43" s="141"/>
+      <c r="S43" s="141"/>
+      <c r="T43" s="141"/>
+      <c r="U43" s="141"/>
+      <c r="V43" s="141"/>
+      <c r="W43" s="141"/>
+      <c r="X43" s="141"/>
       <c r="Y43" s="53" t="s">
         <v>5</v>
       </c>
@@ -18259,33 +18267,33 @@
       <c r="AX43" s="56"/>
     </row>
     <row r="44" spans="1:50" s="29" customFormat="1" ht="42" customHeight="1">
-      <c r="B44" s="139">
+      <c r="B44" s="147">
         <v>1</v>
       </c>
-      <c r="C44" s="139"/>
-      <c r="D44" s="140" t="s">
+      <c r="C44" s="147"/>
+      <c r="D44" s="146" t="s">
         <v>115</v>
       </c>
-      <c r="E44" s="140"/>
-      <c r="F44" s="140"/>
-      <c r="G44" s="140"/>
-      <c r="H44" s="140"/>
-      <c r="I44" s="140"/>
-      <c r="J44" s="140"/>
-      <c r="K44" s="140"/>
-      <c r="L44" s="140"/>
-      <c r="M44" s="140"/>
-      <c r="N44" s="140"/>
-      <c r="O44" s="140"/>
-      <c r="P44" s="140"/>
-      <c r="Q44" s="140"/>
-      <c r="R44" s="140"/>
-      <c r="S44" s="140"/>
-      <c r="T44" s="140"/>
-      <c r="U44" s="140"/>
-      <c r="V44" s="140"/>
-      <c r="W44" s="140"/>
-      <c r="X44" s="140"/>
+      <c r="E44" s="146"/>
+      <c r="F44" s="146"/>
+      <c r="G44" s="146"/>
+      <c r="H44" s="146"/>
+      <c r="I44" s="146"/>
+      <c r="J44" s="146"/>
+      <c r="K44" s="146"/>
+      <c r="L44" s="146"/>
+      <c r="M44" s="146"/>
+      <c r="N44" s="146"/>
+      <c r="O44" s="146"/>
+      <c r="P44" s="146"/>
+      <c r="Q44" s="146"/>
+      <c r="R44" s="146"/>
+      <c r="S44" s="146"/>
+      <c r="T44" s="146"/>
+      <c r="U44" s="146"/>
+      <c r="V44" s="146"/>
+      <c r="W44" s="146"/>
+      <c r="X44" s="146"/>
       <c r="Y44" s="70" t="s">
         <v>116</v>
       </c>
@@ -18316,67 +18324,67 @@
       <c r="AX44" s="72"/>
     </row>
     <row r="45" spans="1:50" s="29" customFormat="1" ht="40.5" customHeight="1">
-      <c r="B45" s="139">
+      <c r="B45" s="147">
         <v>2</v>
       </c>
-      <c r="C45" s="139"/>
-      <c r="D45" s="140" t="s">
+      <c r="C45" s="147"/>
+      <c r="D45" s="146" t="s">
         <v>117</v>
       </c>
-      <c r="E45" s="140"/>
-      <c r="F45" s="140"/>
-      <c r="G45" s="140"/>
-      <c r="H45" s="140"/>
-      <c r="I45" s="140"/>
-      <c r="J45" s="140"/>
-      <c r="K45" s="140"/>
-      <c r="L45" s="140"/>
-      <c r="M45" s="140"/>
-      <c r="N45" s="140"/>
-      <c r="O45" s="140"/>
-      <c r="P45" s="140"/>
-      <c r="Q45" s="140"/>
-      <c r="R45" s="140"/>
-      <c r="S45" s="140"/>
-      <c r="T45" s="140"/>
-      <c r="U45" s="140"/>
-      <c r="V45" s="140"/>
-      <c r="W45" s="140"/>
-      <c r="X45" s="140"/>
-      <c r="Y45" s="140" t="s">
+      <c r="E45" s="146"/>
+      <c r="F45" s="146"/>
+      <c r="G45" s="146"/>
+      <c r="H45" s="146"/>
+      <c r="I45" s="146"/>
+      <c r="J45" s="146"/>
+      <c r="K45" s="146"/>
+      <c r="L45" s="146"/>
+      <c r="M45" s="146"/>
+      <c r="N45" s="146"/>
+      <c r="O45" s="146"/>
+      <c r="P45" s="146"/>
+      <c r="Q45" s="146"/>
+      <c r="R45" s="146"/>
+      <c r="S45" s="146"/>
+      <c r="T45" s="146"/>
+      <c r="U45" s="146"/>
+      <c r="V45" s="146"/>
+      <c r="W45" s="146"/>
+      <c r="X45" s="146"/>
+      <c r="Y45" s="146" t="s">
         <v>118</v>
       </c>
-      <c r="Z45" s="140"/>
-      <c r="AA45" s="140"/>
-      <c r="AB45" s="140"/>
-      <c r="AC45" s="140"/>
-      <c r="AD45" s="140"/>
-      <c r="AE45" s="140"/>
-      <c r="AF45" s="140"/>
-      <c r="AG45" s="140"/>
-      <c r="AH45" s="140"/>
-      <c r="AI45" s="140"/>
-      <c r="AJ45" s="140"/>
-      <c r="AK45" s="140"/>
-      <c r="AL45" s="140"/>
-      <c r="AM45" s="140"/>
-      <c r="AN45" s="140"/>
-      <c r="AO45" s="140"/>
-      <c r="AP45" s="140"/>
-      <c r="AQ45" s="140"/>
-      <c r="AR45" s="140"/>
-      <c r="AS45" s="140"/>
-      <c r="AT45" s="140"/>
-      <c r="AU45" s="140"/>
-      <c r="AV45" s="140"/>
-      <c r="AW45" s="140"/>
-      <c r="AX45" s="140"/>
+      <c r="Z45" s="146"/>
+      <c r="AA45" s="146"/>
+      <c r="AB45" s="146"/>
+      <c r="AC45" s="146"/>
+      <c r="AD45" s="146"/>
+      <c r="AE45" s="146"/>
+      <c r="AF45" s="146"/>
+      <c r="AG45" s="146"/>
+      <c r="AH45" s="146"/>
+      <c r="AI45" s="146"/>
+      <c r="AJ45" s="146"/>
+      <c r="AK45" s="146"/>
+      <c r="AL45" s="146"/>
+      <c r="AM45" s="146"/>
+      <c r="AN45" s="146"/>
+      <c r="AO45" s="146"/>
+      <c r="AP45" s="146"/>
+      <c r="AQ45" s="146"/>
+      <c r="AR45" s="146"/>
+      <c r="AS45" s="146"/>
+      <c r="AT45" s="146"/>
+      <c r="AU45" s="146"/>
+      <c r="AV45" s="146"/>
+      <c r="AW45" s="146"/>
+      <c r="AX45" s="146"/>
     </row>
     <row r="46" spans="1:50" s="29" customFormat="1">
-      <c r="B46" s="139">
+      <c r="B46" s="147">
         <v>3</v>
       </c>
-      <c r="C46" s="139"/>
+      <c r="C46" s="147"/>
       <c r="D46" s="73"/>
       <c r="E46" s="74"/>
       <c r="F46" s="74"/>
@@ -18426,10 +18434,10 @@
       <c r="AX46" s="76"/>
     </row>
     <row r="47" spans="1:50" s="29" customFormat="1">
-      <c r="B47" s="139">
+      <c r="B47" s="147">
         <v>4</v>
       </c>
-      <c r="C47" s="139"/>
+      <c r="C47" s="147"/>
       <c r="D47" s="73"/>
       <c r="E47" s="74"/>
       <c r="F47" s="74"/>
@@ -18479,10 +18487,10 @@
       <c r="AX47" s="76"/>
     </row>
     <row r="48" spans="1:50" s="29" customFormat="1">
-      <c r="B48" s="139">
+      <c r="B48" s="147">
         <v>5</v>
       </c>
-      <c r="C48" s="139"/>
+      <c r="C48" s="147"/>
       <c r="D48" s="73"/>
       <c r="E48" s="74"/>
       <c r="F48" s="74"/>
@@ -18532,10 +18540,10 @@
       <c r="AX48" s="76"/>
     </row>
     <row r="49" spans="1:50" s="29" customFormat="1">
-      <c r="B49" s="139">
+      <c r="B49" s="147">
         <v>6</v>
       </c>
-      <c r="C49" s="139"/>
+      <c r="C49" s="147"/>
       <c r="D49" s="73"/>
       <c r="E49" s="74"/>
       <c r="F49" s="74"/>
@@ -18585,10 +18593,10 @@
       <c r="AX49" s="76"/>
     </row>
     <row r="50" spans="1:50" s="29" customFormat="1">
-      <c r="B50" s="139">
+      <c r="B50" s="147">
         <v>7</v>
       </c>
-      <c r="C50" s="139"/>
+      <c r="C50" s="147"/>
       <c r="D50" s="73"/>
       <c r="E50" s="74"/>
       <c r="F50" s="74"/>
@@ -18639,10 +18647,10 @@
     </row>
     <row r="51" spans="1:50">
       <c r="A51" s="29"/>
-      <c r="B51" s="139">
+      <c r="B51" s="147">
         <v>8</v>
       </c>
-      <c r="C51" s="139"/>
+      <c r="C51" s="147"/>
       <c r="D51" s="73"/>
       <c r="E51" s="74"/>
       <c r="F51" s="74"/>
@@ -18693,6 +18701,22 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:X45"/>
+    <mergeCell ref="Y45:AX45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:X43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:X44"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B3:AW4"/>
     <mergeCell ref="B17:C17"/>
@@ -18706,22 +18730,6 @@
     <mergeCell ref="K19:AB19"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="Y45:AX45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:X43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:X44"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:X45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -20964,338 +20972,338 @@
     </row>
     <row r="13" spans="1:50" s="29" customFormat="1"/>
     <row r="14" spans="1:50" s="29" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B14" s="142" t="s">
+      <c r="B14" s="141" t="s">
         <v>169</v>
       </c>
-      <c r="C14" s="142"/>
-      <c r="D14" s="156" t="s">
+      <c r="C14" s="141"/>
+      <c r="D14" s="154" t="s">
         <v>170</v>
       </c>
-      <c r="E14" s="156"/>
-      <c r="F14" s="156"/>
-      <c r="G14" s="156"/>
-      <c r="H14" s="156"/>
-      <c r="I14" s="156"/>
-      <c r="J14" s="156"/>
-      <c r="K14" s="156"/>
-      <c r="L14" s="156"/>
-      <c r="M14" s="156"/>
-      <c r="N14" s="142" t="s">
+      <c r="E14" s="154"/>
+      <c r="F14" s="154"/>
+      <c r="G14" s="154"/>
+      <c r="H14" s="154"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="154"/>
+      <c r="K14" s="154"/>
+      <c r="L14" s="154"/>
+      <c r="M14" s="154"/>
+      <c r="N14" s="141" t="s">
         <v>171</v>
       </c>
-      <c r="O14" s="142"/>
-      <c r="P14" s="142"/>
-      <c r="Q14" s="142"/>
-      <c r="R14" s="142"/>
-      <c r="S14" s="142"/>
-      <c r="T14" s="142"/>
-      <c r="U14" s="142"/>
-      <c r="V14" s="142"/>
-      <c r="W14" s="142"/>
-      <c r="X14" s="142"/>
-      <c r="Y14" s="142"/>
-      <c r="Z14" s="142"/>
-      <c r="AA14" s="142"/>
-      <c r="AB14" s="142"/>
-      <c r="AC14" s="142"/>
-      <c r="AD14" s="142" t="s">
+      <c r="O14" s="141"/>
+      <c r="P14" s="141"/>
+      <c r="Q14" s="141"/>
+      <c r="R14" s="141"/>
+      <c r="S14" s="141"/>
+      <c r="T14" s="141"/>
+      <c r="U14" s="141"/>
+      <c r="V14" s="141"/>
+      <c r="W14" s="141"/>
+      <c r="X14" s="141"/>
+      <c r="Y14" s="141"/>
+      <c r="Z14" s="141"/>
+      <c r="AA14" s="141"/>
+      <c r="AB14" s="141"/>
+      <c r="AC14" s="141"/>
+      <c r="AD14" s="141" t="s">
         <v>172</v>
       </c>
-      <c r="AE14" s="142"/>
-      <c r="AF14" s="142"/>
-      <c r="AG14" s="142"/>
-      <c r="AH14" s="142"/>
-      <c r="AI14" s="142"/>
-      <c r="AJ14" s="142"/>
-      <c r="AK14" s="142" t="s">
+      <c r="AE14" s="141"/>
+      <c r="AF14" s="141"/>
+      <c r="AG14" s="141"/>
+      <c r="AH14" s="141"/>
+      <c r="AI14" s="141"/>
+      <c r="AJ14" s="141"/>
+      <c r="AK14" s="141" t="s">
         <v>173</v>
       </c>
-      <c r="AL14" s="142"/>
-      <c r="AM14" s="142"/>
-      <c r="AN14" s="142"/>
-      <c r="AO14" s="142"/>
-      <c r="AP14" s="142"/>
-      <c r="AQ14" s="142" t="s">
+      <c r="AL14" s="141"/>
+      <c r="AM14" s="141"/>
+      <c r="AN14" s="141"/>
+      <c r="AO14" s="141"/>
+      <c r="AP14" s="141"/>
+      <c r="AQ14" s="141" t="s">
         <v>174</v>
       </c>
-      <c r="AR14" s="142"/>
-      <c r="AS14" s="142"/>
-      <c r="AT14" s="142" t="s">
+      <c r="AR14" s="141"/>
+      <c r="AS14" s="141"/>
+      <c r="AT14" s="141" t="s">
         <v>175</v>
       </c>
-      <c r="AU14" s="142"/>
-      <c r="AV14" s="142"/>
-      <c r="AW14" s="142"/>
+      <c r="AU14" s="141"/>
+      <c r="AV14" s="141"/>
+      <c r="AW14" s="141"/>
     </row>
     <row r="15" spans="1:50" s="88" customFormat="1" ht="30" customHeight="1">
-      <c r="B15" s="151">
+      <c r="B15" s="150">
         <v>1</v>
       </c>
-      <c r="C15" s="151"/>
-      <c r="D15" s="153" t="s">
+      <c r="C15" s="150"/>
+      <c r="D15" s="151" t="s">
         <v>176</v>
       </c>
-      <c r="E15" s="153"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="153"/>
-      <c r="I15" s="153"/>
-      <c r="J15" s="153"/>
-      <c r="K15" s="153"/>
-      <c r="L15" s="153"/>
-      <c r="M15" s="153"/>
-      <c r="N15" s="140" t="s">
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="151"/>
+      <c r="M15" s="151"/>
+      <c r="N15" s="146" t="s">
         <v>177</v>
       </c>
-      <c r="O15" s="140"/>
-      <c r="P15" s="140"/>
-      <c r="Q15" s="140"/>
-      <c r="R15" s="140"/>
-      <c r="S15" s="140"/>
-      <c r="T15" s="140"/>
-      <c r="U15" s="140"/>
-      <c r="V15" s="140"/>
-      <c r="W15" s="140"/>
-      <c r="X15" s="140"/>
-      <c r="Y15" s="140"/>
-      <c r="Z15" s="140"/>
-      <c r="AA15" s="140"/>
-      <c r="AB15" s="140"/>
-      <c r="AC15" s="140"/>
-      <c r="AD15" s="153" t="s">
+      <c r="O15" s="146"/>
+      <c r="P15" s="146"/>
+      <c r="Q15" s="146"/>
+      <c r="R15" s="146"/>
+      <c r="S15" s="146"/>
+      <c r="T15" s="146"/>
+      <c r="U15" s="146"/>
+      <c r="V15" s="146"/>
+      <c r="W15" s="146"/>
+      <c r="X15" s="146"/>
+      <c r="Y15" s="146"/>
+      <c r="Z15" s="146"/>
+      <c r="AA15" s="146"/>
+      <c r="AB15" s="146"/>
+      <c r="AC15" s="146"/>
+      <c r="AD15" s="151" t="s">
         <v>178</v>
       </c>
-      <c r="AE15" s="153"/>
-      <c r="AF15" s="153"/>
-      <c r="AG15" s="153"/>
-      <c r="AH15" s="153"/>
-      <c r="AI15" s="153"/>
-      <c r="AJ15" s="153"/>
-      <c r="AK15" s="153" t="s">
+      <c r="AE15" s="151"/>
+      <c r="AF15" s="151"/>
+      <c r="AG15" s="151"/>
+      <c r="AH15" s="151"/>
+      <c r="AI15" s="151"/>
+      <c r="AJ15" s="151"/>
+      <c r="AK15" s="151" t="s">
         <v>179</v>
       </c>
-      <c r="AL15" s="153"/>
-      <c r="AM15" s="153"/>
-      <c r="AN15" s="153"/>
-      <c r="AO15" s="153"/>
-      <c r="AP15" s="153"/>
-      <c r="AQ15" s="154">
+      <c r="AL15" s="151"/>
+      <c r="AM15" s="151"/>
+      <c r="AN15" s="151"/>
+      <c r="AO15" s="151"/>
+      <c r="AP15" s="151"/>
+      <c r="AQ15" s="152">
         <v>4</v>
       </c>
-      <c r="AR15" s="154"/>
-      <c r="AS15" s="154"/>
-      <c r="AT15" s="155"/>
-      <c r="AU15" s="155"/>
-      <c r="AV15" s="155"/>
-      <c r="AW15" s="155"/>
+      <c r="AR15" s="152"/>
+      <c r="AS15" s="152"/>
+      <c r="AT15" s="153"/>
+      <c r="AU15" s="153"/>
+      <c r="AV15" s="153"/>
+      <c r="AW15" s="153"/>
     </row>
     <row r="16" spans="1:50" s="88" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B16" s="151">
+      <c r="B16" s="150">
         <v>2</v>
       </c>
-      <c r="C16" s="151"/>
-      <c r="D16" s="152"/>
-      <c r="E16" s="152"/>
-      <c r="F16" s="152"/>
-      <c r="G16" s="152"/>
-      <c r="H16" s="152"/>
-      <c r="I16" s="152"/>
-      <c r="J16" s="152"/>
-      <c r="K16" s="152"/>
-      <c r="L16" s="152"/>
-      <c r="M16" s="152"/>
-      <c r="N16" s="152"/>
-      <c r="O16" s="152"/>
-      <c r="P16" s="152"/>
-      <c r="Q16" s="152"/>
-      <c r="R16" s="152"/>
-      <c r="S16" s="152"/>
-      <c r="T16" s="152"/>
-      <c r="U16" s="152"/>
-      <c r="V16" s="152"/>
-      <c r="W16" s="152"/>
-      <c r="X16" s="152"/>
-      <c r="Y16" s="152"/>
-      <c r="Z16" s="152"/>
-      <c r="AA16" s="152"/>
-      <c r="AB16" s="152"/>
-      <c r="AC16" s="152"/>
-      <c r="AD16" s="152"/>
-      <c r="AE16" s="152"/>
-      <c r="AF16" s="152"/>
-      <c r="AG16" s="152"/>
-      <c r="AH16" s="152"/>
-      <c r="AI16" s="152"/>
-      <c r="AJ16" s="152"/>
-      <c r="AK16" s="152"/>
-      <c r="AL16" s="152"/>
-      <c r="AM16" s="152"/>
-      <c r="AN16" s="152"/>
-      <c r="AO16" s="152"/>
-      <c r="AP16" s="152"/>
-      <c r="AQ16" s="151"/>
-      <c r="AR16" s="151"/>
-      <c r="AS16" s="151"/>
-      <c r="AT16" s="150"/>
-      <c r="AU16" s="150"/>
-      <c r="AV16" s="150"/>
-      <c r="AW16" s="150"/>
+      <c r="C16" s="150"/>
+      <c r="D16" s="156"/>
+      <c r="E16" s="156"/>
+      <c r="F16" s="156"/>
+      <c r="G16" s="156"/>
+      <c r="H16" s="156"/>
+      <c r="I16" s="156"/>
+      <c r="J16" s="156"/>
+      <c r="K16" s="156"/>
+      <c r="L16" s="156"/>
+      <c r="M16" s="156"/>
+      <c r="N16" s="156"/>
+      <c r="O16" s="156"/>
+      <c r="P16" s="156"/>
+      <c r="Q16" s="156"/>
+      <c r="R16" s="156"/>
+      <c r="S16" s="156"/>
+      <c r="T16" s="156"/>
+      <c r="U16" s="156"/>
+      <c r="V16" s="156"/>
+      <c r="W16" s="156"/>
+      <c r="X16" s="156"/>
+      <c r="Y16" s="156"/>
+      <c r="Z16" s="156"/>
+      <c r="AA16" s="156"/>
+      <c r="AB16" s="156"/>
+      <c r="AC16" s="156"/>
+      <c r="AD16" s="156"/>
+      <c r="AE16" s="156"/>
+      <c r="AF16" s="156"/>
+      <c r="AG16" s="156"/>
+      <c r="AH16" s="156"/>
+      <c r="AI16" s="156"/>
+      <c r="AJ16" s="156"/>
+      <c r="AK16" s="156"/>
+      <c r="AL16" s="156"/>
+      <c r="AM16" s="156"/>
+      <c r="AN16" s="156"/>
+      <c r="AO16" s="156"/>
+      <c r="AP16" s="156"/>
+      <c r="AQ16" s="150"/>
+      <c r="AR16" s="150"/>
+      <c r="AS16" s="150"/>
+      <c r="AT16" s="155"/>
+      <c r="AU16" s="155"/>
+      <c r="AV16" s="155"/>
+      <c r="AW16" s="155"/>
     </row>
     <row r="17" spans="1:50" s="88" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B17" s="151">
+      <c r="B17" s="150">
         <v>3</v>
       </c>
-      <c r="C17" s="151"/>
-      <c r="D17" s="152"/>
-      <c r="E17" s="152"/>
-      <c r="F17" s="152"/>
-      <c r="G17" s="152"/>
-      <c r="H17" s="152"/>
-      <c r="I17" s="152"/>
-      <c r="J17" s="152"/>
-      <c r="K17" s="152"/>
-      <c r="L17" s="152"/>
-      <c r="M17" s="152"/>
-      <c r="N17" s="152"/>
-      <c r="O17" s="152"/>
-      <c r="P17" s="152"/>
-      <c r="Q17" s="152"/>
-      <c r="R17" s="152"/>
-      <c r="S17" s="152"/>
-      <c r="T17" s="152"/>
-      <c r="U17" s="152"/>
-      <c r="V17" s="152"/>
-      <c r="W17" s="152"/>
-      <c r="X17" s="152"/>
-      <c r="Y17" s="152"/>
-      <c r="Z17" s="152"/>
-      <c r="AA17" s="152"/>
-      <c r="AB17" s="152"/>
-      <c r="AC17" s="152"/>
-      <c r="AD17" s="152"/>
-      <c r="AE17" s="152"/>
-      <c r="AF17" s="152"/>
-      <c r="AG17" s="152"/>
-      <c r="AH17" s="152"/>
-      <c r="AI17" s="152"/>
-      <c r="AJ17" s="152"/>
-      <c r="AK17" s="152"/>
-      <c r="AL17" s="152"/>
-      <c r="AM17" s="152"/>
-      <c r="AN17" s="152"/>
-      <c r="AO17" s="152"/>
-      <c r="AP17" s="152"/>
-      <c r="AQ17" s="151"/>
-      <c r="AR17" s="151"/>
-      <c r="AS17" s="151"/>
-      <c r="AT17" s="150"/>
-      <c r="AU17" s="150"/>
-      <c r="AV17" s="150"/>
-      <c r="AW17" s="150"/>
+      <c r="C17" s="150"/>
+      <c r="D17" s="156"/>
+      <c r="E17" s="156"/>
+      <c r="F17" s="156"/>
+      <c r="G17" s="156"/>
+      <c r="H17" s="156"/>
+      <c r="I17" s="156"/>
+      <c r="J17" s="156"/>
+      <c r="K17" s="156"/>
+      <c r="L17" s="156"/>
+      <c r="M17" s="156"/>
+      <c r="N17" s="156"/>
+      <c r="O17" s="156"/>
+      <c r="P17" s="156"/>
+      <c r="Q17" s="156"/>
+      <c r="R17" s="156"/>
+      <c r="S17" s="156"/>
+      <c r="T17" s="156"/>
+      <c r="U17" s="156"/>
+      <c r="V17" s="156"/>
+      <c r="W17" s="156"/>
+      <c r="X17" s="156"/>
+      <c r="Y17" s="156"/>
+      <c r="Z17" s="156"/>
+      <c r="AA17" s="156"/>
+      <c r="AB17" s="156"/>
+      <c r="AC17" s="156"/>
+      <c r="AD17" s="156"/>
+      <c r="AE17" s="156"/>
+      <c r="AF17" s="156"/>
+      <c r="AG17" s="156"/>
+      <c r="AH17" s="156"/>
+      <c r="AI17" s="156"/>
+      <c r="AJ17" s="156"/>
+      <c r="AK17" s="156"/>
+      <c r="AL17" s="156"/>
+      <c r="AM17" s="156"/>
+      <c r="AN17" s="156"/>
+      <c r="AO17" s="156"/>
+      <c r="AP17" s="156"/>
+      <c r="AQ17" s="150"/>
+      <c r="AR17" s="150"/>
+      <c r="AS17" s="150"/>
+      <c r="AT17" s="155"/>
+      <c r="AU17" s="155"/>
+      <c r="AV17" s="155"/>
+      <c r="AW17" s="155"/>
     </row>
     <row r="18" spans="1:50" s="88" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B18" s="151">
+      <c r="B18" s="150">
         <v>4</v>
       </c>
-      <c r="C18" s="151"/>
-      <c r="D18" s="152"/>
-      <c r="E18" s="152"/>
-      <c r="F18" s="152"/>
-      <c r="G18" s="152"/>
-      <c r="H18" s="152"/>
-      <c r="I18" s="152"/>
-      <c r="J18" s="152"/>
-      <c r="K18" s="152"/>
-      <c r="L18" s="152"/>
-      <c r="M18" s="152"/>
-      <c r="N18" s="152"/>
-      <c r="O18" s="152"/>
-      <c r="P18" s="152"/>
-      <c r="Q18" s="152"/>
-      <c r="R18" s="152"/>
-      <c r="S18" s="152"/>
-      <c r="T18" s="152"/>
-      <c r="U18" s="152"/>
-      <c r="V18" s="152"/>
-      <c r="W18" s="152"/>
-      <c r="X18" s="152"/>
-      <c r="Y18" s="152"/>
-      <c r="Z18" s="152"/>
-      <c r="AA18" s="152"/>
-      <c r="AB18" s="152"/>
-      <c r="AC18" s="152"/>
-      <c r="AD18" s="152"/>
-      <c r="AE18" s="152"/>
-      <c r="AF18" s="152"/>
-      <c r="AG18" s="152"/>
-      <c r="AH18" s="152"/>
-      <c r="AI18" s="152"/>
-      <c r="AJ18" s="152"/>
-      <c r="AK18" s="152"/>
-      <c r="AL18" s="152"/>
-      <c r="AM18" s="152"/>
-      <c r="AN18" s="152"/>
-      <c r="AO18" s="152"/>
-      <c r="AP18" s="152"/>
-      <c r="AQ18" s="151"/>
-      <c r="AR18" s="151"/>
-      <c r="AS18" s="151"/>
-      <c r="AT18" s="150"/>
-      <c r="AU18" s="150"/>
-      <c r="AV18" s="150"/>
-      <c r="AW18" s="150"/>
+      <c r="C18" s="150"/>
+      <c r="D18" s="156"/>
+      <c r="E18" s="156"/>
+      <c r="F18" s="156"/>
+      <c r="G18" s="156"/>
+      <c r="H18" s="156"/>
+      <c r="I18" s="156"/>
+      <c r="J18" s="156"/>
+      <c r="K18" s="156"/>
+      <c r="L18" s="156"/>
+      <c r="M18" s="156"/>
+      <c r="N18" s="156"/>
+      <c r="O18" s="156"/>
+      <c r="P18" s="156"/>
+      <c r="Q18" s="156"/>
+      <c r="R18" s="156"/>
+      <c r="S18" s="156"/>
+      <c r="T18" s="156"/>
+      <c r="U18" s="156"/>
+      <c r="V18" s="156"/>
+      <c r="W18" s="156"/>
+      <c r="X18" s="156"/>
+      <c r="Y18" s="156"/>
+      <c r="Z18" s="156"/>
+      <c r="AA18" s="156"/>
+      <c r="AB18" s="156"/>
+      <c r="AC18" s="156"/>
+      <c r="AD18" s="156"/>
+      <c r="AE18" s="156"/>
+      <c r="AF18" s="156"/>
+      <c r="AG18" s="156"/>
+      <c r="AH18" s="156"/>
+      <c r="AI18" s="156"/>
+      <c r="AJ18" s="156"/>
+      <c r="AK18" s="156"/>
+      <c r="AL18" s="156"/>
+      <c r="AM18" s="156"/>
+      <c r="AN18" s="156"/>
+      <c r="AO18" s="156"/>
+      <c r="AP18" s="156"/>
+      <c r="AQ18" s="150"/>
+      <c r="AR18" s="150"/>
+      <c r="AS18" s="150"/>
+      <c r="AT18" s="155"/>
+      <c r="AU18" s="155"/>
+      <c r="AV18" s="155"/>
+      <c r="AW18" s="155"/>
     </row>
     <row r="19" spans="1:50" s="88" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B19" s="151">
+      <c r="B19" s="150">
         <v>5</v>
       </c>
-      <c r="C19" s="151"/>
-      <c r="D19" s="152"/>
-      <c r="E19" s="152"/>
-      <c r="F19" s="152"/>
-      <c r="G19" s="152"/>
-      <c r="H19" s="152"/>
-      <c r="I19" s="152"/>
-      <c r="J19" s="152"/>
-      <c r="K19" s="152"/>
-      <c r="L19" s="152"/>
-      <c r="M19" s="152"/>
-      <c r="N19" s="152"/>
-      <c r="O19" s="152"/>
-      <c r="P19" s="152"/>
-      <c r="Q19" s="152"/>
-      <c r="R19" s="152"/>
-      <c r="S19" s="152"/>
-      <c r="T19" s="152"/>
-      <c r="U19" s="152"/>
-      <c r="V19" s="152"/>
-      <c r="W19" s="152"/>
-      <c r="X19" s="152"/>
-      <c r="Y19" s="152"/>
-      <c r="Z19" s="152"/>
-      <c r="AA19" s="152"/>
-      <c r="AB19" s="152"/>
-      <c r="AC19" s="152"/>
-      <c r="AD19" s="152"/>
-      <c r="AE19" s="152"/>
-      <c r="AF19" s="152"/>
-      <c r="AG19" s="152"/>
-      <c r="AH19" s="152"/>
-      <c r="AI19" s="152"/>
-      <c r="AJ19" s="152"/>
-      <c r="AK19" s="152"/>
-      <c r="AL19" s="152"/>
-      <c r="AM19" s="152"/>
-      <c r="AN19" s="152"/>
-      <c r="AO19" s="152"/>
-      <c r="AP19" s="152"/>
-      <c r="AQ19" s="151"/>
-      <c r="AR19" s="151"/>
-      <c r="AS19" s="151"/>
-      <c r="AT19" s="150"/>
-      <c r="AU19" s="150"/>
-      <c r="AV19" s="150"/>
-      <c r="AW19" s="150"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="156"/>
+      <c r="E19" s="156"/>
+      <c r="F19" s="156"/>
+      <c r="G19" s="156"/>
+      <c r="H19" s="156"/>
+      <c r="I19" s="156"/>
+      <c r="J19" s="156"/>
+      <c r="K19" s="156"/>
+      <c r="L19" s="156"/>
+      <c r="M19" s="156"/>
+      <c r="N19" s="156"/>
+      <c r="O19" s="156"/>
+      <c r="P19" s="156"/>
+      <c r="Q19" s="156"/>
+      <c r="R19" s="156"/>
+      <c r="S19" s="156"/>
+      <c r="T19" s="156"/>
+      <c r="U19" s="156"/>
+      <c r="V19" s="156"/>
+      <c r="W19" s="156"/>
+      <c r="X19" s="156"/>
+      <c r="Y19" s="156"/>
+      <c r="Z19" s="156"/>
+      <c r="AA19" s="156"/>
+      <c r="AB19" s="156"/>
+      <c r="AC19" s="156"/>
+      <c r="AD19" s="156"/>
+      <c r="AE19" s="156"/>
+      <c r="AF19" s="156"/>
+      <c r="AG19" s="156"/>
+      <c r="AH19" s="156"/>
+      <c r="AI19" s="156"/>
+      <c r="AJ19" s="156"/>
+      <c r="AK19" s="156"/>
+      <c r="AL19" s="156"/>
+      <c r="AM19" s="156"/>
+      <c r="AN19" s="156"/>
+      <c r="AO19" s="156"/>
+      <c r="AP19" s="156"/>
+      <c r="AQ19" s="150"/>
+      <c r="AR19" s="150"/>
+      <c r="AS19" s="150"/>
+      <c r="AT19" s="155"/>
+      <c r="AU19" s="155"/>
+      <c r="AV19" s="155"/>
+      <c r="AW19" s="155"/>
     </row>
     <row r="20" spans="1:50" s="29" customFormat="1"/>
     <row r="21" spans="1:50" s="29" customFormat="1">
@@ -21463,6 +21471,34 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="AT18:AW18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:M19"/>
+    <mergeCell ref="N19:AC19"/>
+    <mergeCell ref="AD19:AJ19"/>
+    <mergeCell ref="AK19:AP19"/>
+    <mergeCell ref="AQ19:AS19"/>
+    <mergeCell ref="AT19:AW19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:M18"/>
+    <mergeCell ref="N18:AC18"/>
+    <mergeCell ref="AD18:AJ18"/>
+    <mergeCell ref="AK18:AP18"/>
+    <mergeCell ref="AQ18:AS18"/>
+    <mergeCell ref="AT16:AW16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:M17"/>
+    <mergeCell ref="N17:AC17"/>
+    <mergeCell ref="AD17:AJ17"/>
+    <mergeCell ref="AK17:AP17"/>
+    <mergeCell ref="AQ17:AS17"/>
+    <mergeCell ref="AT17:AW17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:M16"/>
+    <mergeCell ref="N16:AC16"/>
+    <mergeCell ref="AD16:AJ16"/>
+    <mergeCell ref="AK16:AP16"/>
+    <mergeCell ref="AQ16:AS16"/>
     <mergeCell ref="AT14:AW14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:M15"/>
@@ -21477,34 +21513,6 @@
     <mergeCell ref="AD14:AJ14"/>
     <mergeCell ref="AK14:AP14"/>
     <mergeCell ref="AQ14:AS14"/>
-    <mergeCell ref="AT16:AW16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:M17"/>
-    <mergeCell ref="N17:AC17"/>
-    <mergeCell ref="AD17:AJ17"/>
-    <mergeCell ref="AK17:AP17"/>
-    <mergeCell ref="AQ17:AS17"/>
-    <mergeCell ref="AT17:AW17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:M16"/>
-    <mergeCell ref="N16:AC16"/>
-    <mergeCell ref="AD16:AJ16"/>
-    <mergeCell ref="AK16:AP16"/>
-    <mergeCell ref="AQ16:AS16"/>
-    <mergeCell ref="AT18:AW18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:M19"/>
-    <mergeCell ref="N19:AC19"/>
-    <mergeCell ref="AD19:AJ19"/>
-    <mergeCell ref="AK19:AP19"/>
-    <mergeCell ref="AQ19:AS19"/>
-    <mergeCell ref="AT19:AW19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:M18"/>
-    <mergeCell ref="N18:AC18"/>
-    <mergeCell ref="AD18:AJ18"/>
-    <mergeCell ref="AK18:AP18"/>
-    <mergeCell ref="AQ18:AS18"/>
   </mergeCells>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -22329,83 +22337,83 @@
       </c>
     </row>
     <row r="21" spans="1:50" s="28" customFormat="1" ht="14.25" customHeight="1">
-      <c r="B21" s="142" t="s">
+      <c r="B21" s="141" t="s">
         <v>169</v>
       </c>
-      <c r="C21" s="142"/>
-      <c r="D21" s="142" t="s">
+      <c r="C21" s="141"/>
+      <c r="D21" s="141" t="s">
         <v>198</v>
       </c>
-      <c r="E21" s="142"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="142"/>
-      <c r="H21" s="142"/>
-      <c r="I21" s="142"/>
-      <c r="J21" s="142"/>
-      <c r="K21" s="142" t="s">
+      <c r="E21" s="141"/>
+      <c r="F21" s="141"/>
+      <c r="G21" s="141"/>
+      <c r="H21" s="141"/>
+      <c r="I21" s="141"/>
+      <c r="J21" s="141"/>
+      <c r="K21" s="141" t="s">
         <v>199</v>
       </c>
-      <c r="L21" s="142"/>
-      <c r="M21" s="142"/>
-      <c r="N21" s="142"/>
-      <c r="O21" s="142"/>
-      <c r="P21" s="142"/>
-      <c r="Q21" s="142" t="s">
+      <c r="L21" s="141"/>
+      <c r="M21" s="141"/>
+      <c r="N21" s="141"/>
+      <c r="O21" s="141"/>
+      <c r="P21" s="141"/>
+      <c r="Q21" s="141" t="s">
         <v>200</v>
       </c>
-      <c r="R21" s="142"/>
-      <c r="S21" s="142"/>
-      <c r="T21" s="142"/>
-      <c r="U21" s="142"/>
-      <c r="V21" s="142"/>
-      <c r="W21" s="142"/>
-      <c r="X21" s="142" t="s">
+      <c r="R21" s="141"/>
+      <c r="S21" s="141"/>
+      <c r="T21" s="141"/>
+      <c r="U21" s="141"/>
+      <c r="V21" s="141"/>
+      <c r="W21" s="141"/>
+      <c r="X21" s="141" t="s">
         <v>201</v>
       </c>
-      <c r="Y21" s="142"/>
-      <c r="Z21" s="142"/>
-      <c r="AA21" s="142"/>
-      <c r="AB21" s="142"/>
-      <c r="AC21" s="142" t="s">
+      <c r="Y21" s="141"/>
+      <c r="Z21" s="141"/>
+      <c r="AA21" s="141"/>
+      <c r="AB21" s="141"/>
+      <c r="AC21" s="141" t="s">
         <v>202</v>
       </c>
-      <c r="AD21" s="142"/>
-      <c r="AE21" s="142"/>
-      <c r="AF21" s="142"/>
-      <c r="AG21" s="142"/>
-      <c r="AH21" s="142" t="s">
+      <c r="AD21" s="141"/>
+      <c r="AE21" s="141"/>
+      <c r="AF21" s="141"/>
+      <c r="AG21" s="141"/>
+      <c r="AH21" s="141" t="s">
         <v>203</v>
       </c>
-      <c r="AI21" s="142"/>
-      <c r="AJ21" s="142"/>
-      <c r="AK21" s="142"/>
-      <c r="AL21" s="142"/>
-      <c r="AM21" s="142"/>
-      <c r="AN21" s="142" t="s">
+      <c r="AI21" s="141"/>
+      <c r="AJ21" s="141"/>
+      <c r="AK21" s="141"/>
+      <c r="AL21" s="141"/>
+      <c r="AM21" s="141"/>
+      <c r="AN21" s="141" t="s">
         <v>204</v>
       </c>
-      <c r="AO21" s="142"/>
-      <c r="AP21" s="142"/>
-      <c r="AQ21" s="142"/>
-      <c r="AR21" s="142"/>
-      <c r="AS21" s="142"/>
-      <c r="AT21" s="142"/>
-      <c r="AU21" s="142"/>
-      <c r="AV21" s="142"/>
-      <c r="AW21" s="142"/>
+      <c r="AO21" s="141"/>
+      <c r="AP21" s="141"/>
+      <c r="AQ21" s="141"/>
+      <c r="AR21" s="141"/>
+      <c r="AS21" s="141"/>
+      <c r="AT21" s="141"/>
+      <c r="AU21" s="141"/>
+      <c r="AV21" s="141"/>
+      <c r="AW21" s="141"/>
     </row>
     <row r="22" spans="1:50" s="49" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B22" s="157" t="s">
+      <c r="B22" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="157"/>
-      <c r="D22" s="161"/>
-      <c r="E22" s="161"/>
-      <c r="F22" s="161"/>
-      <c r="G22" s="161"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="161"/>
-      <c r="J22" s="161"/>
+      <c r="C22" s="159"/>
+      <c r="D22" s="160"/>
+      <c r="E22" s="160"/>
+      <c r="F22" s="160"/>
+      <c r="G22" s="160"/>
+      <c r="H22" s="160"/>
+      <c r="I22" s="160"/>
+      <c r="J22" s="160"/>
       <c r="K22" s="158" t="s">
         <v>205</v>
       </c>
@@ -22414,33 +22422,33 @@
       <c r="N22" s="158"/>
       <c r="O22" s="158"/>
       <c r="P22" s="158"/>
-      <c r="Q22" s="164"/>
-      <c r="R22" s="164"/>
-      <c r="S22" s="164"/>
-      <c r="T22" s="164"/>
-      <c r="U22" s="164"/>
-      <c r="V22" s="164"/>
-      <c r="W22" s="164"/>
-      <c r="X22" s="160" t="s">
+      <c r="Q22" s="161"/>
+      <c r="R22" s="161"/>
+      <c r="S22" s="161"/>
+      <c r="T22" s="161"/>
+      <c r="U22" s="161"/>
+      <c r="V22" s="161"/>
+      <c r="W22" s="161"/>
+      <c r="X22" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="Y22" s="160"/>
-      <c r="Z22" s="160"/>
-      <c r="AA22" s="160"/>
-      <c r="AB22" s="160"/>
-      <c r="AC22" s="160" t="s">
+      <c r="Y22" s="162"/>
+      <c r="Z22" s="162"/>
+      <c r="AA22" s="162"/>
+      <c r="AB22" s="162"/>
+      <c r="AC22" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AD22" s="160"/>
-      <c r="AE22" s="160"/>
-      <c r="AF22" s="160"/>
-      <c r="AG22" s="160"/>
-      <c r="AH22" s="163"/>
-      <c r="AI22" s="163"/>
-      <c r="AJ22" s="163"/>
-      <c r="AK22" s="163"/>
-      <c r="AL22" s="163"/>
-      <c r="AM22" s="163"/>
+      <c r="AD22" s="162"/>
+      <c r="AE22" s="162"/>
+      <c r="AF22" s="162"/>
+      <c r="AG22" s="162"/>
+      <c r="AH22" s="157"/>
+      <c r="AI22" s="157"/>
+      <c r="AJ22" s="157"/>
+      <c r="AK22" s="157"/>
+      <c r="AL22" s="157"/>
+      <c r="AM22" s="157"/>
       <c r="AN22" s="158"/>
       <c r="AO22" s="158"/>
       <c r="AP22" s="158"/>
@@ -22453,17 +22461,17 @@
       <c r="AW22" s="158"/>
     </row>
     <row r="23" spans="1:50" s="49" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B23" s="157" t="s">
+      <c r="B23" s="159" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="157"/>
-      <c r="D23" s="161"/>
-      <c r="E23" s="161"/>
-      <c r="F23" s="161"/>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161"/>
-      <c r="J23" s="161"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="160"/>
+      <c r="E23" s="160"/>
+      <c r="F23" s="160"/>
+      <c r="G23" s="160"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="160"/>
+      <c r="J23" s="160"/>
       <c r="K23" s="158" t="s">
         <v>179</v>
       </c>
@@ -22472,33 +22480,33 @@
       <c r="N23" s="158"/>
       <c r="O23" s="158"/>
       <c r="P23" s="158"/>
-      <c r="Q23" s="164"/>
-      <c r="R23" s="164"/>
-      <c r="S23" s="164"/>
-      <c r="T23" s="164"/>
-      <c r="U23" s="164"/>
-      <c r="V23" s="164"/>
-      <c r="W23" s="164"/>
-      <c r="X23" s="160" t="s">
+      <c r="Q23" s="161"/>
+      <c r="R23" s="161"/>
+      <c r="S23" s="161"/>
+      <c r="T23" s="161"/>
+      <c r="U23" s="161"/>
+      <c r="V23" s="161"/>
+      <c r="W23" s="161"/>
+      <c r="X23" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="Y23" s="160"/>
-      <c r="Z23" s="160"/>
-      <c r="AA23" s="160"/>
-      <c r="AB23" s="160"/>
-      <c r="AC23" s="160" t="s">
+      <c r="Y23" s="162"/>
+      <c r="Z23" s="162"/>
+      <c r="AA23" s="162"/>
+      <c r="AB23" s="162"/>
+      <c r="AC23" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AD23" s="160"/>
-      <c r="AE23" s="160"/>
-      <c r="AF23" s="160"/>
-      <c r="AG23" s="160"/>
-      <c r="AH23" s="163"/>
-      <c r="AI23" s="163"/>
-      <c r="AJ23" s="163"/>
-      <c r="AK23" s="163"/>
-      <c r="AL23" s="163"/>
-      <c r="AM23" s="163"/>
+      <c r="AD23" s="162"/>
+      <c r="AE23" s="162"/>
+      <c r="AF23" s="162"/>
+      <c r="AG23" s="162"/>
+      <c r="AH23" s="157"/>
+      <c r="AI23" s="157"/>
+      <c r="AJ23" s="157"/>
+      <c r="AK23" s="157"/>
+      <c r="AL23" s="157"/>
+      <c r="AM23" s="157"/>
       <c r="AN23" s="158"/>
       <c r="AO23" s="158"/>
       <c r="AP23" s="158"/>
@@ -22511,10 +22519,10 @@
       <c r="AW23" s="158"/>
     </row>
     <row r="24" spans="1:50" s="49" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B24" s="157" t="s">
+      <c r="B24" s="159" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="157"/>
+      <c r="C24" s="159"/>
       <c r="D24" s="158"/>
       <c r="E24" s="158"/>
       <c r="F24" s="158"/>
@@ -22530,33 +22538,33 @@
       <c r="N24" s="158"/>
       <c r="O24" s="158"/>
       <c r="P24" s="158"/>
-      <c r="Q24" s="164"/>
-      <c r="R24" s="164"/>
-      <c r="S24" s="164"/>
-      <c r="T24" s="164"/>
-      <c r="U24" s="164"/>
-      <c r="V24" s="164"/>
-      <c r="W24" s="164"/>
-      <c r="X24" s="160" t="s">
+      <c r="Q24" s="161"/>
+      <c r="R24" s="161"/>
+      <c r="S24" s="161"/>
+      <c r="T24" s="161"/>
+      <c r="U24" s="161"/>
+      <c r="V24" s="161"/>
+      <c r="W24" s="161"/>
+      <c r="X24" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="Y24" s="160"/>
-      <c r="Z24" s="160"/>
-      <c r="AA24" s="160"/>
-      <c r="AB24" s="160"/>
-      <c r="AC24" s="160" t="s">
+      <c r="Y24" s="162"/>
+      <c r="Z24" s="162"/>
+      <c r="AA24" s="162"/>
+      <c r="AB24" s="162"/>
+      <c r="AC24" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AD24" s="160"/>
-      <c r="AE24" s="160"/>
-      <c r="AF24" s="160"/>
-      <c r="AG24" s="160"/>
-      <c r="AH24" s="163"/>
-      <c r="AI24" s="163"/>
-      <c r="AJ24" s="163"/>
-      <c r="AK24" s="163"/>
-      <c r="AL24" s="163"/>
-      <c r="AM24" s="163"/>
+      <c r="AD24" s="162"/>
+      <c r="AE24" s="162"/>
+      <c r="AF24" s="162"/>
+      <c r="AG24" s="162"/>
+      <c r="AH24" s="157"/>
+      <c r="AI24" s="157"/>
+      <c r="AJ24" s="157"/>
+      <c r="AK24" s="157"/>
+      <c r="AL24" s="157"/>
+      <c r="AM24" s="157"/>
       <c r="AN24" s="158"/>
       <c r="AO24" s="158"/>
       <c r="AP24" s="158"/>
@@ -22569,10 +22577,10 @@
       <c r="AW24" s="158"/>
     </row>
     <row r="25" spans="1:50" s="49" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B25" s="157" t="s">
+      <c r="B25" s="159" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="157"/>
+      <c r="C25" s="159"/>
       <c r="D25" s="158"/>
       <c r="E25" s="158"/>
       <c r="F25" s="158"/>
@@ -22588,33 +22596,33 @@
       <c r="N25" s="158"/>
       <c r="O25" s="158"/>
       <c r="P25" s="158"/>
-      <c r="Q25" s="164"/>
-      <c r="R25" s="164"/>
-      <c r="S25" s="164"/>
-      <c r="T25" s="164"/>
-      <c r="U25" s="164"/>
-      <c r="V25" s="164"/>
-      <c r="W25" s="164"/>
-      <c r="X25" s="160" t="s">
+      <c r="Q25" s="161"/>
+      <c r="R25" s="161"/>
+      <c r="S25" s="161"/>
+      <c r="T25" s="161"/>
+      <c r="U25" s="161"/>
+      <c r="V25" s="161"/>
+      <c r="W25" s="161"/>
+      <c r="X25" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="Y25" s="160"/>
-      <c r="Z25" s="160"/>
-      <c r="AA25" s="160"/>
-      <c r="AB25" s="160"/>
-      <c r="AC25" s="160" t="s">
+      <c r="Y25" s="162"/>
+      <c r="Z25" s="162"/>
+      <c r="AA25" s="162"/>
+      <c r="AB25" s="162"/>
+      <c r="AC25" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AD25" s="160"/>
-      <c r="AE25" s="160"/>
-      <c r="AF25" s="160"/>
-      <c r="AG25" s="160"/>
-      <c r="AH25" s="163"/>
-      <c r="AI25" s="163"/>
-      <c r="AJ25" s="163"/>
-      <c r="AK25" s="163"/>
-      <c r="AL25" s="163"/>
-      <c r="AM25" s="163"/>
+      <c r="AD25" s="162"/>
+      <c r="AE25" s="162"/>
+      <c r="AF25" s="162"/>
+      <c r="AG25" s="162"/>
+      <c r="AH25" s="157"/>
+      <c r="AI25" s="157"/>
+      <c r="AJ25" s="157"/>
+      <c r="AK25" s="157"/>
+      <c r="AL25" s="157"/>
+      <c r="AM25" s="157"/>
       <c r="AN25" s="158"/>
       <c r="AO25" s="158"/>
       <c r="AP25" s="158"/>
@@ -22632,196 +22640,196 @@
       </c>
     </row>
     <row r="28" spans="1:50">
-      <c r="B28" s="142" t="s">
+      <c r="B28" s="141" t="s">
         <v>169</v>
       </c>
-      <c r="C28" s="142"/>
-      <c r="D28" s="142" t="s">
+      <c r="C28" s="141"/>
+      <c r="D28" s="141" t="s">
         <v>209</v>
       </c>
-      <c r="E28" s="142"/>
-      <c r="F28" s="142"/>
-      <c r="G28" s="142"/>
-      <c r="H28" s="142"/>
-      <c r="I28" s="142"/>
-      <c r="J28" s="142"/>
-      <c r="K28" s="142" t="s">
+      <c r="E28" s="141"/>
+      <c r="F28" s="141"/>
+      <c r="G28" s="141"/>
+      <c r="H28" s="141"/>
+      <c r="I28" s="141"/>
+      <c r="J28" s="141"/>
+      <c r="K28" s="141" t="s">
         <v>199</v>
       </c>
-      <c r="L28" s="142"/>
-      <c r="M28" s="142"/>
-      <c r="N28" s="142"/>
-      <c r="O28" s="142"/>
-      <c r="P28" s="142"/>
-      <c r="Q28" s="142" t="s">
+      <c r="L28" s="141"/>
+      <c r="M28" s="141"/>
+      <c r="N28" s="141"/>
+      <c r="O28" s="141"/>
+      <c r="P28" s="141"/>
+      <c r="Q28" s="141" t="s">
         <v>210</v>
       </c>
-      <c r="R28" s="142"/>
-      <c r="S28" s="142"/>
-      <c r="T28" s="142"/>
-      <c r="U28" s="142"/>
-      <c r="V28" s="142"/>
-      <c r="W28" s="142"/>
-      <c r="X28" s="142"/>
-      <c r="Y28" s="142"/>
-      <c r="Z28" s="142"/>
-      <c r="AA28" s="142"/>
-      <c r="AB28" s="142"/>
-      <c r="AC28" s="142"/>
-      <c r="AD28" s="142"/>
-      <c r="AE28" s="142"/>
-      <c r="AF28" s="142"/>
-      <c r="AG28" s="142"/>
-      <c r="AH28" s="142" t="s">
+      <c r="R28" s="141"/>
+      <c r="S28" s="141"/>
+      <c r="T28" s="141"/>
+      <c r="U28" s="141"/>
+      <c r="V28" s="141"/>
+      <c r="W28" s="141"/>
+      <c r="X28" s="141"/>
+      <c r="Y28" s="141"/>
+      <c r="Z28" s="141"/>
+      <c r="AA28" s="141"/>
+      <c r="AB28" s="141"/>
+      <c r="AC28" s="141"/>
+      <c r="AD28" s="141"/>
+      <c r="AE28" s="141"/>
+      <c r="AF28" s="141"/>
+      <c r="AG28" s="141"/>
+      <c r="AH28" s="141" t="s">
         <v>201</v>
       </c>
-      <c r="AI28" s="142"/>
-      <c r="AJ28" s="142"/>
-      <c r="AK28" s="142"/>
-      <c r="AL28" s="142"/>
-      <c r="AM28" s="142" t="s">
+      <c r="AI28" s="141"/>
+      <c r="AJ28" s="141"/>
+      <c r="AK28" s="141"/>
+      <c r="AL28" s="141"/>
+      <c r="AM28" s="141" t="s">
         <v>202</v>
       </c>
-      <c r="AN28" s="142"/>
-      <c r="AO28" s="142"/>
-      <c r="AP28" s="142"/>
-      <c r="AQ28" s="142"/>
-      <c r="AR28" s="142" t="s">
+      <c r="AN28" s="141"/>
+      <c r="AO28" s="141"/>
+      <c r="AP28" s="141"/>
+      <c r="AQ28" s="141"/>
+      <c r="AR28" s="141" t="s">
         <v>211</v>
       </c>
-      <c r="AS28" s="142"/>
-      <c r="AT28" s="142"/>
-      <c r="AU28" s="142"/>
-      <c r="AV28" s="142"/>
-      <c r="AW28" s="142"/>
+      <c r="AS28" s="141"/>
+      <c r="AT28" s="141"/>
+      <c r="AU28" s="141"/>
+      <c r="AV28" s="141"/>
+      <c r="AW28" s="141"/>
     </row>
     <row r="29" spans="1:50" ht="14.25">
-      <c r="B29" s="157" t="s">
+      <c r="B29" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="157"/>
-      <c r="D29" s="161" t="s">
+      <c r="C29" s="159"/>
+      <c r="D29" s="160" t="s">
         <v>212</v>
       </c>
-      <c r="E29" s="161"/>
-      <c r="F29" s="161"/>
-      <c r="G29" s="161"/>
-      <c r="H29" s="161"/>
-      <c r="I29" s="161"/>
-      <c r="J29" s="161"/>
-      <c r="K29" s="161" t="s">
+      <c r="E29" s="160"/>
+      <c r="F29" s="160"/>
+      <c r="G29" s="160"/>
+      <c r="H29" s="160"/>
+      <c r="I29" s="160"/>
+      <c r="J29" s="160"/>
+      <c r="K29" s="160" t="s">
         <v>213</v>
       </c>
-      <c r="L29" s="161"/>
-      <c r="M29" s="161"/>
-      <c r="N29" s="161"/>
-      <c r="O29" s="161"/>
-      <c r="P29" s="161"/>
-      <c r="Q29" s="162" t="s">
+      <c r="L29" s="160"/>
+      <c r="M29" s="160"/>
+      <c r="N29" s="160"/>
+      <c r="O29" s="160"/>
+      <c r="P29" s="160"/>
+      <c r="Q29" s="163" t="s">
         <v>214</v>
       </c>
-      <c r="R29" s="162"/>
-      <c r="S29" s="162"/>
-      <c r="T29" s="162"/>
-      <c r="U29" s="162"/>
-      <c r="V29" s="162"/>
-      <c r="W29" s="162"/>
-      <c r="X29" s="162"/>
-      <c r="Y29" s="162"/>
-      <c r="Z29" s="162"/>
-      <c r="AA29" s="162"/>
-      <c r="AB29" s="162"/>
-      <c r="AC29" s="162"/>
-      <c r="AD29" s="162"/>
-      <c r="AE29" s="162"/>
-      <c r="AF29" s="162"/>
-      <c r="AG29" s="162"/>
-      <c r="AH29" s="160" t="s">
+      <c r="R29" s="163"/>
+      <c r="S29" s="163"/>
+      <c r="T29" s="163"/>
+      <c r="U29" s="163"/>
+      <c r="V29" s="163"/>
+      <c r="W29" s="163"/>
+      <c r="X29" s="163"/>
+      <c r="Y29" s="163"/>
+      <c r="Z29" s="163"/>
+      <c r="AA29" s="163"/>
+      <c r="AB29" s="163"/>
+      <c r="AC29" s="163"/>
+      <c r="AD29" s="163"/>
+      <c r="AE29" s="163"/>
+      <c r="AF29" s="163"/>
+      <c r="AG29" s="163"/>
+      <c r="AH29" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AI29" s="160"/>
-      <c r="AJ29" s="160"/>
-      <c r="AK29" s="160"/>
-      <c r="AL29" s="160"/>
-      <c r="AM29" s="160" t="s">
+      <c r="AI29" s="162"/>
+      <c r="AJ29" s="162"/>
+      <c r="AK29" s="162"/>
+      <c r="AL29" s="162"/>
+      <c r="AM29" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AN29" s="160"/>
-      <c r="AO29" s="160"/>
-      <c r="AP29" s="160"/>
-      <c r="AQ29" s="160"/>
-      <c r="AR29" s="157" t="s">
+      <c r="AN29" s="162"/>
+      <c r="AO29" s="162"/>
+      <c r="AP29" s="162"/>
+      <c r="AQ29" s="162"/>
+      <c r="AR29" s="159" t="s">
         <v>215</v>
       </c>
-      <c r="AS29" s="157"/>
-      <c r="AT29" s="157"/>
-      <c r="AU29" s="157"/>
-      <c r="AV29" s="157"/>
-      <c r="AW29" s="157"/>
+      <c r="AS29" s="159"/>
+      <c r="AT29" s="159"/>
+      <c r="AU29" s="159"/>
+      <c r="AV29" s="159"/>
+      <c r="AW29" s="159"/>
     </row>
     <row r="30" spans="1:50" ht="14.25">
-      <c r="B30" s="157" t="s">
+      <c r="B30" s="159" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="157"/>
-      <c r="D30" s="161" t="s">
+      <c r="C30" s="159"/>
+      <c r="D30" s="160" t="s">
         <v>216</v>
       </c>
-      <c r="E30" s="161"/>
-      <c r="F30" s="161"/>
-      <c r="G30" s="161"/>
-      <c r="H30" s="161"/>
-      <c r="I30" s="161"/>
-      <c r="J30" s="161"/>
+      <c r="E30" s="160"/>
+      <c r="F30" s="160"/>
+      <c r="G30" s="160"/>
+      <c r="H30" s="160"/>
+      <c r="I30" s="160"/>
+      <c r="J30" s="160"/>
       <c r="K30" s="158"/>
       <c r="L30" s="158"/>
       <c r="M30" s="158"/>
       <c r="N30" s="158"/>
       <c r="O30" s="158"/>
       <c r="P30" s="158"/>
-      <c r="Q30" s="159"/>
-      <c r="R30" s="159"/>
-      <c r="S30" s="159"/>
-      <c r="T30" s="159"/>
-      <c r="U30" s="159"/>
-      <c r="V30" s="159"/>
-      <c r="W30" s="159"/>
-      <c r="X30" s="159"/>
-      <c r="Y30" s="159"/>
-      <c r="Z30" s="159"/>
-      <c r="AA30" s="159"/>
-      <c r="AB30" s="159"/>
-      <c r="AC30" s="159"/>
-      <c r="AD30" s="159"/>
-      <c r="AE30" s="159"/>
-      <c r="AF30" s="159"/>
-      <c r="AG30" s="159"/>
-      <c r="AH30" s="160" t="s">
+      <c r="Q30" s="164"/>
+      <c r="R30" s="164"/>
+      <c r="S30" s="164"/>
+      <c r="T30" s="164"/>
+      <c r="U30" s="164"/>
+      <c r="V30" s="164"/>
+      <c r="W30" s="164"/>
+      <c r="X30" s="164"/>
+      <c r="Y30" s="164"/>
+      <c r="Z30" s="164"/>
+      <c r="AA30" s="164"/>
+      <c r="AB30" s="164"/>
+      <c r="AC30" s="164"/>
+      <c r="AD30" s="164"/>
+      <c r="AE30" s="164"/>
+      <c r="AF30" s="164"/>
+      <c r="AG30" s="164"/>
+      <c r="AH30" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AI30" s="160"/>
-      <c r="AJ30" s="160"/>
-      <c r="AK30" s="160"/>
-      <c r="AL30" s="160"/>
-      <c r="AM30" s="160" t="s">
+      <c r="AI30" s="162"/>
+      <c r="AJ30" s="162"/>
+      <c r="AK30" s="162"/>
+      <c r="AL30" s="162"/>
+      <c r="AM30" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AN30" s="160"/>
-      <c r="AO30" s="160"/>
-      <c r="AP30" s="160"/>
-      <c r="AQ30" s="160"/>
-      <c r="AR30" s="157"/>
-      <c r="AS30" s="157"/>
-      <c r="AT30" s="157"/>
-      <c r="AU30" s="157"/>
-      <c r="AV30" s="157"/>
-      <c r="AW30" s="157"/>
+      <c r="AN30" s="162"/>
+      <c r="AO30" s="162"/>
+      <c r="AP30" s="162"/>
+      <c r="AQ30" s="162"/>
+      <c r="AR30" s="159"/>
+      <c r="AS30" s="159"/>
+      <c r="AT30" s="159"/>
+      <c r="AU30" s="159"/>
+      <c r="AV30" s="159"/>
+      <c r="AW30" s="159"/>
     </row>
     <row r="31" spans="1:50" ht="14.25">
-      <c r="B31" s="157" t="s">
+      <c r="B31" s="159" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="157"/>
+      <c r="C31" s="159"/>
       <c r="D31" s="158"/>
       <c r="E31" s="158"/>
       <c r="F31" s="158"/>
@@ -22835,49 +22843,49 @@
       <c r="N31" s="158"/>
       <c r="O31" s="158"/>
       <c r="P31" s="158"/>
-      <c r="Q31" s="159"/>
-      <c r="R31" s="159"/>
-      <c r="S31" s="159"/>
-      <c r="T31" s="159"/>
-      <c r="U31" s="159"/>
-      <c r="V31" s="159"/>
-      <c r="W31" s="159"/>
-      <c r="X31" s="159"/>
-      <c r="Y31" s="159"/>
-      <c r="Z31" s="159"/>
-      <c r="AA31" s="159"/>
-      <c r="AB31" s="159"/>
-      <c r="AC31" s="159"/>
-      <c r="AD31" s="159"/>
-      <c r="AE31" s="159"/>
-      <c r="AF31" s="159"/>
-      <c r="AG31" s="159"/>
-      <c r="AH31" s="160" t="s">
+      <c r="Q31" s="164"/>
+      <c r="R31" s="164"/>
+      <c r="S31" s="164"/>
+      <c r="T31" s="164"/>
+      <c r="U31" s="164"/>
+      <c r="V31" s="164"/>
+      <c r="W31" s="164"/>
+      <c r="X31" s="164"/>
+      <c r="Y31" s="164"/>
+      <c r="Z31" s="164"/>
+      <c r="AA31" s="164"/>
+      <c r="AB31" s="164"/>
+      <c r="AC31" s="164"/>
+      <c r="AD31" s="164"/>
+      <c r="AE31" s="164"/>
+      <c r="AF31" s="164"/>
+      <c r="AG31" s="164"/>
+      <c r="AH31" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AI31" s="160"/>
-      <c r="AJ31" s="160"/>
-      <c r="AK31" s="160"/>
-      <c r="AL31" s="160"/>
-      <c r="AM31" s="160" t="s">
+      <c r="AI31" s="162"/>
+      <c r="AJ31" s="162"/>
+      <c r="AK31" s="162"/>
+      <c r="AL31" s="162"/>
+      <c r="AM31" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AN31" s="160"/>
-      <c r="AO31" s="160"/>
-      <c r="AP31" s="160"/>
-      <c r="AQ31" s="160"/>
-      <c r="AR31" s="157"/>
-      <c r="AS31" s="157"/>
-      <c r="AT31" s="157"/>
-      <c r="AU31" s="157"/>
-      <c r="AV31" s="157"/>
-      <c r="AW31" s="157"/>
+      <c r="AN31" s="162"/>
+      <c r="AO31" s="162"/>
+      <c r="AP31" s="162"/>
+      <c r="AQ31" s="162"/>
+      <c r="AR31" s="159"/>
+      <c r="AS31" s="159"/>
+      <c r="AT31" s="159"/>
+      <c r="AU31" s="159"/>
+      <c r="AV31" s="159"/>
+      <c r="AW31" s="159"/>
     </row>
     <row r="32" spans="1:50" ht="14.25">
-      <c r="B32" s="157" t="s">
+      <c r="B32" s="159" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="157"/>
+      <c r="C32" s="159"/>
       <c r="D32" s="158"/>
       <c r="E32" s="158"/>
       <c r="F32" s="158"/>
@@ -22891,49 +22899,49 @@
       <c r="N32" s="158"/>
       <c r="O32" s="158"/>
       <c r="P32" s="158"/>
-      <c r="Q32" s="159"/>
-      <c r="R32" s="159"/>
-      <c r="S32" s="159"/>
-      <c r="T32" s="159"/>
-      <c r="U32" s="159"/>
-      <c r="V32" s="159"/>
-      <c r="W32" s="159"/>
-      <c r="X32" s="159"/>
-      <c r="Y32" s="159"/>
-      <c r="Z32" s="159"/>
-      <c r="AA32" s="159"/>
-      <c r="AB32" s="159"/>
-      <c r="AC32" s="159"/>
-      <c r="AD32" s="159"/>
-      <c r="AE32" s="159"/>
-      <c r="AF32" s="159"/>
-      <c r="AG32" s="159"/>
-      <c r="AH32" s="160" t="s">
+      <c r="Q32" s="164"/>
+      <c r="R32" s="164"/>
+      <c r="S32" s="164"/>
+      <c r="T32" s="164"/>
+      <c r="U32" s="164"/>
+      <c r="V32" s="164"/>
+      <c r="W32" s="164"/>
+      <c r="X32" s="164"/>
+      <c r="Y32" s="164"/>
+      <c r="Z32" s="164"/>
+      <c r="AA32" s="164"/>
+      <c r="AB32" s="164"/>
+      <c r="AC32" s="164"/>
+      <c r="AD32" s="164"/>
+      <c r="AE32" s="164"/>
+      <c r="AF32" s="164"/>
+      <c r="AG32" s="164"/>
+      <c r="AH32" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AI32" s="160"/>
-      <c r="AJ32" s="160"/>
-      <c r="AK32" s="160"/>
-      <c r="AL32" s="160"/>
-      <c r="AM32" s="160" t="s">
+      <c r="AI32" s="162"/>
+      <c r="AJ32" s="162"/>
+      <c r="AK32" s="162"/>
+      <c r="AL32" s="162"/>
+      <c r="AM32" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AN32" s="160"/>
-      <c r="AO32" s="160"/>
-      <c r="AP32" s="160"/>
-      <c r="AQ32" s="160"/>
-      <c r="AR32" s="157"/>
-      <c r="AS32" s="157"/>
-      <c r="AT32" s="157"/>
-      <c r="AU32" s="157"/>
-      <c r="AV32" s="157"/>
-      <c r="AW32" s="157"/>
+      <c r="AN32" s="162"/>
+      <c r="AO32" s="162"/>
+      <c r="AP32" s="162"/>
+      <c r="AQ32" s="162"/>
+      <c r="AR32" s="159"/>
+      <c r="AS32" s="159"/>
+      <c r="AT32" s="159"/>
+      <c r="AU32" s="159"/>
+      <c r="AV32" s="159"/>
+      <c r="AW32" s="159"/>
     </row>
     <row r="33" spans="2:49" ht="14.25">
-      <c r="B33" s="157" t="s">
+      <c r="B33" s="159" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="157"/>
+      <c r="C33" s="159"/>
       <c r="D33" s="158"/>
       <c r="E33" s="158"/>
       <c r="F33" s="158"/>
@@ -22947,55 +22955,104 @@
       <c r="N33" s="158"/>
       <c r="O33" s="158"/>
       <c r="P33" s="158"/>
-      <c r="Q33" s="159"/>
-      <c r="R33" s="159"/>
-      <c r="S33" s="159"/>
-      <c r="T33" s="159"/>
-      <c r="U33" s="159"/>
-      <c r="V33" s="159"/>
-      <c r="W33" s="159"/>
-      <c r="X33" s="159"/>
-      <c r="Y33" s="159"/>
-      <c r="Z33" s="159"/>
-      <c r="AA33" s="159"/>
-      <c r="AB33" s="159"/>
-      <c r="AC33" s="159"/>
-      <c r="AD33" s="159"/>
-      <c r="AE33" s="159"/>
-      <c r="AF33" s="159"/>
-      <c r="AG33" s="159"/>
-      <c r="AH33" s="160" t="s">
+      <c r="Q33" s="164"/>
+      <c r="R33" s="164"/>
+      <c r="S33" s="164"/>
+      <c r="T33" s="164"/>
+      <c r="U33" s="164"/>
+      <c r="V33" s="164"/>
+      <c r="W33" s="164"/>
+      <c r="X33" s="164"/>
+      <c r="Y33" s="164"/>
+      <c r="Z33" s="164"/>
+      <c r="AA33" s="164"/>
+      <c r="AB33" s="164"/>
+      <c r="AC33" s="164"/>
+      <c r="AD33" s="164"/>
+      <c r="AE33" s="164"/>
+      <c r="AF33" s="164"/>
+      <c r="AG33" s="164"/>
+      <c r="AH33" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AI33" s="160"/>
-      <c r="AJ33" s="160"/>
-      <c r="AK33" s="160"/>
-      <c r="AL33" s="160"/>
-      <c r="AM33" s="160" t="s">
+      <c r="AI33" s="162"/>
+      <c r="AJ33" s="162"/>
+      <c r="AK33" s="162"/>
+      <c r="AL33" s="162"/>
+      <c r="AM33" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="AN33" s="160"/>
-      <c r="AO33" s="160"/>
-      <c r="AP33" s="160"/>
-      <c r="AQ33" s="160"/>
-      <c r="AR33" s="157"/>
-      <c r="AS33" s="157"/>
-      <c r="AT33" s="157"/>
-      <c r="AU33" s="157"/>
-      <c r="AV33" s="157"/>
-      <c r="AW33" s="157"/>
+      <c r="AN33" s="162"/>
+      <c r="AO33" s="162"/>
+      <c r="AP33" s="162"/>
+      <c r="AQ33" s="162"/>
+      <c r="AR33" s="159"/>
+      <c r="AS33" s="159"/>
+      <c r="AT33" s="159"/>
+      <c r="AU33" s="159"/>
+      <c r="AV33" s="159"/>
+      <c r="AW33" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="C6:AW9"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="K21:P21"/>
-    <mergeCell ref="Q21:W21"/>
-    <mergeCell ref="X21:AB21"/>
-    <mergeCell ref="AC21:AG21"/>
-    <mergeCell ref="AH21:AM21"/>
-    <mergeCell ref="AN21:AW21"/>
+    <mergeCell ref="AR32:AW32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="K33:P33"/>
+    <mergeCell ref="Q33:AG33"/>
+    <mergeCell ref="AH33:AL33"/>
+    <mergeCell ref="AM33:AQ33"/>
+    <mergeCell ref="AR33:AW33"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:J32"/>
+    <mergeCell ref="K32:P32"/>
+    <mergeCell ref="Q32:AG32"/>
+    <mergeCell ref="AH32:AL32"/>
+    <mergeCell ref="AM32:AQ32"/>
+    <mergeCell ref="AR30:AW30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="K31:P31"/>
+    <mergeCell ref="Q31:AG31"/>
+    <mergeCell ref="AH31:AL31"/>
+    <mergeCell ref="AM31:AQ31"/>
+    <mergeCell ref="AR31:AW31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:J30"/>
+    <mergeCell ref="K30:P30"/>
+    <mergeCell ref="Q30:AG30"/>
+    <mergeCell ref="AH30:AL30"/>
+    <mergeCell ref="AM30:AQ30"/>
+    <mergeCell ref="AR28:AW28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="K29:P29"/>
+    <mergeCell ref="Q29:AG29"/>
+    <mergeCell ref="AH29:AL29"/>
+    <mergeCell ref="AM29:AQ29"/>
+    <mergeCell ref="AR29:AW29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:J28"/>
+    <mergeCell ref="K28:P28"/>
+    <mergeCell ref="Q28:AG28"/>
+    <mergeCell ref="AH28:AL28"/>
+    <mergeCell ref="AM28:AQ28"/>
+    <mergeCell ref="AH24:AM24"/>
+    <mergeCell ref="AN24:AW24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:J25"/>
+    <mergeCell ref="K25:P25"/>
+    <mergeCell ref="Q25:W25"/>
+    <mergeCell ref="X25:AB25"/>
+    <mergeCell ref="AC25:AG25"/>
+    <mergeCell ref="AH25:AM25"/>
+    <mergeCell ref="AN25:AW25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:J24"/>
+    <mergeCell ref="K24:P24"/>
+    <mergeCell ref="Q24:W24"/>
+    <mergeCell ref="X24:AB24"/>
+    <mergeCell ref="AC24:AG24"/>
     <mergeCell ref="AH22:AM22"/>
     <mergeCell ref="AN22:AW22"/>
     <mergeCell ref="B23:C23"/>
@@ -23012,64 +23069,15 @@
     <mergeCell ref="Q22:W22"/>
     <mergeCell ref="X22:AB22"/>
     <mergeCell ref="AC22:AG22"/>
-    <mergeCell ref="AH24:AM24"/>
-    <mergeCell ref="AN24:AW24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:J25"/>
-    <mergeCell ref="K25:P25"/>
-    <mergeCell ref="Q25:W25"/>
-    <mergeCell ref="X25:AB25"/>
-    <mergeCell ref="AC25:AG25"/>
-    <mergeCell ref="AH25:AM25"/>
-    <mergeCell ref="AN25:AW25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:J24"/>
-    <mergeCell ref="K24:P24"/>
-    <mergeCell ref="Q24:W24"/>
-    <mergeCell ref="X24:AB24"/>
-    <mergeCell ref="AC24:AG24"/>
-    <mergeCell ref="AR28:AW28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="K29:P29"/>
-    <mergeCell ref="Q29:AG29"/>
-    <mergeCell ref="AH29:AL29"/>
-    <mergeCell ref="AM29:AQ29"/>
-    <mergeCell ref="AR29:AW29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:J28"/>
-    <mergeCell ref="K28:P28"/>
-    <mergeCell ref="Q28:AG28"/>
-    <mergeCell ref="AH28:AL28"/>
-    <mergeCell ref="AM28:AQ28"/>
-    <mergeCell ref="AR30:AW30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="K31:P31"/>
-    <mergeCell ref="Q31:AG31"/>
-    <mergeCell ref="AH31:AL31"/>
-    <mergeCell ref="AM31:AQ31"/>
-    <mergeCell ref="AR31:AW31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:J30"/>
-    <mergeCell ref="K30:P30"/>
-    <mergeCell ref="Q30:AG30"/>
-    <mergeCell ref="AH30:AL30"/>
-    <mergeCell ref="AM30:AQ30"/>
-    <mergeCell ref="AR32:AW32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:J33"/>
-    <mergeCell ref="K33:P33"/>
-    <mergeCell ref="Q33:AG33"/>
-    <mergeCell ref="AH33:AL33"/>
-    <mergeCell ref="AM33:AQ33"/>
-    <mergeCell ref="AR33:AW33"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:J32"/>
-    <mergeCell ref="K32:P32"/>
-    <mergeCell ref="Q32:AG32"/>
-    <mergeCell ref="AH32:AL32"/>
-    <mergeCell ref="AM32:AQ32"/>
+    <mergeCell ref="C6:AW9"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="K21:P21"/>
+    <mergeCell ref="Q21:W21"/>
+    <mergeCell ref="X21:AB21"/>
+    <mergeCell ref="AC21:AG21"/>
+    <mergeCell ref="AH21:AM21"/>
+    <mergeCell ref="AN21:AW21"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AH22:AM25" xr:uid="{00000000-0002-0000-0700-000000000000}">

</xml_diff>